<commit_message>
All 225 weapons are listed
</commit_message>
<xml_diff>
--- a/Documentation/Items.xlsx
+++ b/Documentation/Items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity_Projects\LC_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AADC8A-D9C4-4590-B306-76D80C66616B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34726C8-E37A-47BB-A08D-829B39A96464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="661">
   <si>
     <t>ID</t>
   </si>
@@ -1752,6 +1752,273 @@
   </si>
   <si>
     <t>Rank XII, Upgrades from Naginata + Ahlspiess</t>
+  </si>
+  <si>
+    <t>Mace</t>
+  </si>
+  <si>
+    <t>Gada</t>
+  </si>
+  <si>
+    <t>Pernach</t>
+  </si>
+  <si>
+    <t>Quauhololli</t>
+  </si>
+  <si>
+    <t>Roundhead</t>
+  </si>
+  <si>
+    <t>Sharur</t>
+  </si>
+  <si>
+    <t>Bozdogan</t>
+  </si>
+  <si>
+    <t>Shishpar</t>
+  </si>
+  <si>
+    <t>Shestopyor</t>
+  </si>
+  <si>
+    <t>Marshal Mace</t>
+  </si>
+  <si>
+    <t>Bulava</t>
+  </si>
+  <si>
+    <t>Morning Star</t>
+  </si>
+  <si>
+    <t>War Hammer</t>
+  </si>
+  <si>
+    <t>A heavy, one handed mace, very useful to break armors. Inflicts Break I on impact.</t>
+  </si>
+  <si>
+    <t>A round-shape mace mounted with a spike. Effective as a melee weapon and a magic staff. Increases the effectiveness of healing abilities.</t>
+  </si>
+  <si>
+    <t>Kanabo</t>
+  </si>
+  <si>
+    <t>A long mace with iron stud on the end. Effective at parrying. Inflicts Bleed I on impact.</t>
+  </si>
+  <si>
+    <t>A winged-mace, capable of breaking through heavy plates. Inflicts Break I and Magic Break I on impact.</t>
+  </si>
+  <si>
+    <t>Rank IV, Upgrades from War Hammer</t>
+  </si>
+  <si>
+    <t>A long shaft with a heavy rock, effective at crushing bones. Increases the effectiveness of healing abilities. Inflicts Break I on impact.</t>
+  </si>
+  <si>
+    <t>Rank V, Upgrades from War Hammer + Gada</t>
+  </si>
+  <si>
+    <t>A long staff with a 12 spikes head. Effective at parrying. Inflicts Bleed II on impact.</t>
+  </si>
+  <si>
+    <t>Rank V, Upgrades from Kanabo</t>
+  </si>
+  <si>
+    <t>A winged, black tainted metal mace. Inflicts Break II and Magic Break II on impact.</t>
+  </si>
+  <si>
+    <t>Rank VII, Upgrades from Pernach</t>
+  </si>
+  <si>
+    <t>A mace with eight flanges and a spike. Increases the effectiveness of healing abilities. Inflicts Break III on impact.</t>
+  </si>
+  <si>
+    <t>Rank VIII, Upgrades from Quauhololli</t>
+  </si>
+  <si>
+    <t>A heavy long shaft with a spiky head, combining blunt force and puncture attacks to kill its enemies. Effective at parrying. Inflicts Bleed II and Slow I on impact.</t>
+  </si>
+  <si>
+    <t>Rank VIII, Upgrades from Roundhead</t>
+  </si>
+  <si>
+    <t>A winged, black tainted metal mace. Inflicts Break II and Magic Break II on impact. Also increases the effectiveness of healing abilities.</t>
+  </si>
+  <si>
+    <t>Rank IX, Upgrades from Bozdogan</t>
+  </si>
+  <si>
+    <t>Trench Raiding Club</t>
+  </si>
+  <si>
+    <t>A short wooden spiky club, very effective at disarming opponents. Inflicts Slow II, Bleed II and Break II on impact. Increases critical strike chance.</t>
+  </si>
+  <si>
+    <t>A mace used in religious ceremonies. Significantly increases the effectiveness of healing abilities. Reduces MP costs by 30%.</t>
+  </si>
+  <si>
+    <t>Rank X, Upgrades from Gada</t>
+  </si>
+  <si>
+    <t>A short studded mace, used in close combat. Inflicts Slow II, Bleed II and Break II on impact. Increases critical strike chance. Increases Magic.</t>
+  </si>
+  <si>
+    <t>Rank XI, Upgrades from Trench Raiding Club</t>
+  </si>
+  <si>
+    <t>The smasher of thousands. This enchanted mace can defeat any demon it faces. Significants increases the effectiveness of healing abilities. Reduces MP costs by 30%. Inflicts Break III and Magic Break III on impact.</t>
+  </si>
+  <si>
+    <t>Rank XII, Upgrades from Shestopyor + Marshal Mace</t>
+  </si>
+  <si>
+    <t>Firearm</t>
+  </si>
+  <si>
+    <t>Musket</t>
+  </si>
+  <si>
+    <t>Blunderbluss</t>
+  </si>
+  <si>
+    <t>Arquebus</t>
+  </si>
+  <si>
+    <t>Huochong</t>
+  </si>
+  <si>
+    <t>Lancaster</t>
+  </si>
+  <si>
+    <t>Ribauldequin</t>
+  </si>
+  <si>
+    <t>San Yan Chong</t>
+  </si>
+  <si>
+    <t>Xun Lei Chong</t>
+  </si>
+  <si>
+    <t>Fomalhaut</t>
+  </si>
+  <si>
+    <t>Long gun with fast but unreliable projectile that deals magic damage.</t>
+  </si>
+  <si>
+    <t>An effective, short range firearm. Ineffective at longer range.</t>
+  </si>
+  <si>
+    <t>Long gun with fast but unreliable projectile that deals magic damage. Inflicts Break I on impact.</t>
+  </si>
+  <si>
+    <t>Rank VI, Upgrades from Arquebus</t>
+  </si>
+  <si>
+    <t>Hand cannon. The projectile explodes on hit, dealing magic damage in an area.</t>
+  </si>
+  <si>
+    <t>Tanegashima</t>
+  </si>
+  <si>
+    <t>Rank VII, Upgrades from Blunderbluss</t>
+  </si>
+  <si>
+    <t>A small pistol with great rate of fire and high precision. Capable of shooting 2 bullets in succession.</t>
+  </si>
+  <si>
+    <t>A volley gun that shoots bullets in a cone. The center bullet is aimed at the primary target, while a total of 7 bullets are fired, 3 on each side. Multiple bullets hitting the same target deal 30% damage.</t>
+  </si>
+  <si>
+    <t>Rank VIII, Upgrades from Huochong</t>
+  </si>
+  <si>
+    <t>Three barrel hand cannon. Its projectiles explode on hit, dealing damage in an area. The primary projectile hits the targets, while the 2 other projectiles create a cone shape around the main fire line. Multiple bullets hitting the same target deal 60% damage.</t>
+  </si>
+  <si>
+    <t>Revolving-barrel, spear-combined musket.The 5 cannons of the weapon destroys any armor it faces. Inflicts Break II and Magic Break II on impact.</t>
+  </si>
+  <si>
+    <t>Rank IX, Upgrades from Musket</t>
+  </si>
+  <si>
+    <t>A large, modern rifle with high precision. Its deadly bullets with pierce through any target, dealing damage to all units in their path. Deals 10% reduced damage of each successive enemy hit, up to a minimum of 60%. Inflicts Bleed II on impact.</t>
+  </si>
+  <si>
+    <t>A firearm with slow fire rate and short range. Inflicts Bleed I on impact.</t>
+  </si>
+  <si>
+    <t>Rank XI, Upgrades from Tanegashima</t>
+  </si>
+  <si>
+    <t>Post Mortem</t>
+  </si>
+  <si>
+    <t>Scythe</t>
+  </si>
+  <si>
+    <t>Sickle</t>
+  </si>
+  <si>
+    <t>Khopesh</t>
+  </si>
+  <si>
+    <t>Kama</t>
+  </si>
+  <si>
+    <t>Billhook</t>
+  </si>
+  <si>
+    <t>War Scythe</t>
+  </si>
+  <si>
+    <t>Harpe</t>
+  </si>
+  <si>
+    <t>Omen of Death</t>
+  </si>
+  <si>
+    <t>Omen of Hope</t>
+  </si>
+  <si>
+    <t>A short, curvy blade, used to harvest. Anything.</t>
+  </si>
+  <si>
+    <t>Short sword, capable of pulling an enemy towards its wielder. Holds the ability Attraction.</t>
+  </si>
+  <si>
+    <t>Traditional tool to reap crops. Can also be used as a short range blade. Increases agility. Increases the efficacy of healing items.</t>
+  </si>
+  <si>
+    <t>A short tool with a blade made of carbon. Increases Magic. Increases the efficacy of healing items.</t>
+  </si>
+  <si>
+    <t>Rank V, Upgrades from Khopesh.</t>
+  </si>
+  <si>
+    <t>A long shaft with a curvy, sharp blade. Effective at parrying. Holds the ability Attraction. Follows any action that differs from basic attacks with a basic attack.</t>
+  </si>
+  <si>
+    <t>Rank VII, Upgrades from Billhook + Kama</t>
+  </si>
+  <si>
+    <t>Adamantine blade, known to be wielded by deities. Increases Magic and Agility. Increases the efficacy of healing items and abilities.</t>
+  </si>
+  <si>
+    <t>A large scythe, whose own shadow reaps through its enemies. Increases Darkness damage dealt by 30%. Increases Magic. Basic attacks steal additional health on hit.</t>
+  </si>
+  <si>
+    <t>Rank X</t>
+  </si>
+  <si>
+    <t>A large scythe, whose aura manifests great power and bravery. Increases Holy damage dealt by 30%. Increases Magic. Grants Faith at the start of the battle.</t>
+  </si>
+  <si>
+    <t>The symbol of the gatekeeper between the realms of life and death. Increases Darkness and Holy damage by 30%. Greatly increases Magic. Basic attacks steal additional health on hit. Grants Faith at the start of the battle.</t>
+  </si>
+  <si>
+    <t>Rank XII, Agrid's ultimate weapon. Upgrades from Omen of Death + Omen of Hope</t>
+  </si>
+  <si>
+    <t>Rank III, Upgrades from Sickle</t>
   </si>
 </sst>
 </file>
@@ -2126,10 +2393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE263883-2701-4B73-BA24-C20413007C34}">
-  <dimension ref="B2:F208"/>
+  <dimension ref="B2:F241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="I191" sqref="I191"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="F232" sqref="F232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5575,45 +5842,606 @@
         <v>571</v>
       </c>
     </row>
-    <row r="206" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B206">
-        <v>2000</v>
+        <v>1192</v>
       </c>
       <c r="C206" t="s">
-        <v>116</v>
+        <v>584</v>
       </c>
       <c r="D206" t="s">
-        <v>121</v>
+        <v>572</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="207" spans="2:6" x14ac:dyDescent="0.25">
+        <v>585</v>
+      </c>
+      <c r="F206" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="207" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B207">
-        <v>2001</v>
+        <v>1193</v>
       </c>
       <c r="C207" t="s">
-        <v>117</v>
+        <v>573</v>
       </c>
       <c r="D207" t="s">
-        <v>122</v>
+        <v>572</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>119</v>
+        <v>586</v>
+      </c>
+      <c r="F207" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="208" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B208">
+        <v>1194</v>
+      </c>
+      <c r="C208" t="s">
+        <v>587</v>
+      </c>
+      <c r="D208" t="s">
+        <v>572</v>
+      </c>
+      <c r="E208" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="F208" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="209" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>1195</v>
+      </c>
+      <c r="C209" t="s">
+        <v>574</v>
+      </c>
+      <c r="D209" t="s">
+        <v>572</v>
+      </c>
+      <c r="E209" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="F209" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="210" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>1196</v>
+      </c>
+      <c r="C210" t="s">
+        <v>575</v>
+      </c>
+      <c r="D210" t="s">
+        <v>572</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="F210" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="211" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B211">
+        <v>1197</v>
+      </c>
+      <c r="C211" t="s">
+        <v>576</v>
+      </c>
+      <c r="D211" t="s">
+        <v>572</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="F211" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="212" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B212">
+        <v>1198</v>
+      </c>
+      <c r="C212" t="s">
+        <v>578</v>
+      </c>
+      <c r="D212" t="s">
+        <v>572</v>
+      </c>
+      <c r="E212" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="F212" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="213" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B213">
+        <v>1199</v>
+      </c>
+      <c r="C213" t="s">
+        <v>579</v>
+      </c>
+      <c r="D213" t="s">
+        <v>572</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="F213" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="214" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B214">
+        <v>1200</v>
+      </c>
+      <c r="C214" t="s">
+        <v>583</v>
+      </c>
+      <c r="D214" t="s">
+        <v>572</v>
+      </c>
+      <c r="E214" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="F214" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="215" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B215">
+        <v>1201</v>
+      </c>
+      <c r="C215" t="s">
+        <v>580</v>
+      </c>
+      <c r="D215" t="s">
+        <v>572</v>
+      </c>
+      <c r="E215" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="F215" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="216" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B216">
+        <v>1202</v>
+      </c>
+      <c r="C216" t="s">
+        <v>603</v>
+      </c>
+      <c r="D216" t="s">
+        <v>572</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="F216" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="217" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <v>1203</v>
+      </c>
+      <c r="C217" t="s">
+        <v>581</v>
+      </c>
+      <c r="D217" t="s">
+        <v>572</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="F217" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="218" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B218">
+        <v>1204</v>
+      </c>
+      <c r="C218" t="s">
+        <v>582</v>
+      </c>
+      <c r="D218" t="s">
+        <v>572</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="F218" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="219" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B219">
+        <v>1205</v>
+      </c>
+      <c r="C219" t="s">
+        <v>577</v>
+      </c>
+      <c r="D219" t="s">
+        <v>572</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="F219" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="220" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B220">
+        <v>1206</v>
+      </c>
+      <c r="C220" t="s">
+        <v>614</v>
+      </c>
+      <c r="D220" t="s">
+        <v>611</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="F220" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="221" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B221">
+        <v>1207</v>
+      </c>
+      <c r="C221" t="s">
+        <v>613</v>
+      </c>
+      <c r="D221" t="s">
+        <v>611</v>
+      </c>
+      <c r="E221" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="F221" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="222" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B222">
+        <v>1208</v>
+      </c>
+      <c r="C222" t="s">
+        <v>612</v>
+      </c>
+      <c r="D222" t="s">
+        <v>611</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="F222" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="223" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B223">
+        <v>1209</v>
+      </c>
+      <c r="C223" t="s">
+        <v>615</v>
+      </c>
+      <c r="D223" t="s">
+        <v>611</v>
+      </c>
+      <c r="E223" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="F223" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="224" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B224">
+        <v>1210</v>
+      </c>
+      <c r="C224" t="s">
+        <v>626</v>
+      </c>
+      <c r="D224" t="s">
+        <v>611</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="F224" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="225" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B225">
+        <v>1211</v>
+      </c>
+      <c r="C225" t="s">
+        <v>616</v>
+      </c>
+      <c r="D225" t="s">
+        <v>611</v>
+      </c>
+      <c r="E225" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="F225" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="226" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <v>1212</v>
+      </c>
+      <c r="C226" t="s">
+        <v>617</v>
+      </c>
+      <c r="D226" t="s">
+        <v>611</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="F226" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="227" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B227">
+        <v>1213</v>
+      </c>
+      <c r="C227" t="s">
+        <v>618</v>
+      </c>
+      <c r="D227" t="s">
+        <v>611</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="F227" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="228" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B228">
+        <v>1214</v>
+      </c>
+      <c r="C228" t="s">
+        <v>619</v>
+      </c>
+      <c r="D228" t="s">
+        <v>611</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="F228" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="229" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B229">
+        <v>1215</v>
+      </c>
+      <c r="C229" t="s">
+        <v>620</v>
+      </c>
+      <c r="D229" t="s">
+        <v>611</v>
+      </c>
+      <c r="E229" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="F229" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="230" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B230">
+        <v>1216</v>
+      </c>
+      <c r="C230" t="s">
+        <v>639</v>
+      </c>
+      <c r="D230" t="s">
+        <v>638</v>
+      </c>
+      <c r="E230" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="F230" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="231" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B231">
+        <v>1217</v>
+      </c>
+      <c r="C231" t="s">
+        <v>640</v>
+      </c>
+      <c r="D231" t="s">
+        <v>638</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="F231" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="232" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B232">
+        <v>1218</v>
+      </c>
+      <c r="C232" t="s">
+        <v>641</v>
+      </c>
+      <c r="D232" t="s">
+        <v>638</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="F232" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="233" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B233">
+        <v>1219</v>
+      </c>
+      <c r="C233" t="s">
+        <v>642</v>
+      </c>
+      <c r="D233" t="s">
+        <v>638</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="F233" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="234" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <v>1220</v>
+      </c>
+      <c r="C234" t="s">
+        <v>643</v>
+      </c>
+      <c r="D234" t="s">
+        <v>638</v>
+      </c>
+      <c r="E234" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="F234" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="235" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <v>1221</v>
+      </c>
+      <c r="C235" t="s">
+        <v>644</v>
+      </c>
+      <c r="D235" t="s">
+        <v>638</v>
+      </c>
+      <c r="E235" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="F235" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="236" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <v>1222</v>
+      </c>
+      <c r="C236" t="s">
+        <v>645</v>
+      </c>
+      <c r="D236" t="s">
+        <v>638</v>
+      </c>
+      <c r="E236" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="F236" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="237" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B237">
+        <v>1223</v>
+      </c>
+      <c r="C237" t="s">
+        <v>646</v>
+      </c>
+      <c r="D237" t="s">
+        <v>638</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="F237" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="238" spans="2:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>1224</v>
+      </c>
+      <c r="C238" t="s">
+        <v>637</v>
+      </c>
+      <c r="D238" t="s">
+        <v>638</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="F238" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="239" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B239">
+        <v>2000</v>
+      </c>
+      <c r="C239" t="s">
+        <v>116</v>
+      </c>
+      <c r="D239" t="s">
+        <v>121</v>
+      </c>
+      <c r="E239" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="240" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B240">
+        <v>2001</v>
+      </c>
+      <c r="C240" t="s">
+        <v>117</v>
+      </c>
+      <c r="D240" t="s">
+        <v>122</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="241" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B241">
         <v>2002</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C241" t="s">
         <v>120</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D241" t="s">
         <v>123</v>
       </c>
-      <c r="E208" s="1" t="s">
+      <c r="E241" s="1" t="s">
         <v>124</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Encodage des haches dans le parser
</commit_message>
<xml_diff>
--- a/Documentation/Items.xlsx
+++ b/Documentation/Items.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity_Projects\LC_Unity\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxad\Documents\git_projects\LC_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8164154-0CDA-47EC-B5B2-A1D55CED62AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6B7126-2ABC-4598-9540-CCA2A7D6F599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2392,8 +2392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE263883-2701-4B73-BA24-C20413007C34}">
   <dimension ref="B2:F241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tous les fichiers de base pour les items sont créés, leurs parsers sont créés et les données sont chargées en mémoire au démarrage
</commit_message>
<xml_diff>
--- a/Documentation/Items.xlsx
+++ b/Documentation/Items.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxad\Documents\git_projects\LC_Unity\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity_Projects\LC_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6B7126-2ABC-4598-9540-CCA2A7D6F599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DB1C33-6E05-48F5-B15D-630C6D8AF942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="667">
   <si>
     <t>ID</t>
   </si>
@@ -2016,6 +2016,27 @@
   </si>
   <si>
     <t>Rank III, Upgrades from Sickle</t>
+  </si>
+  <si>
+    <t>Blood Ring</t>
+  </si>
+  <si>
+    <t>Accessory</t>
+  </si>
+  <si>
+    <t>A rind that boosts its owner's maximum HP</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Iron Ore</t>
+  </si>
+  <si>
+    <t>Sealed Medallion</t>
+  </si>
+  <si>
+    <t>Key Item</t>
   </si>
 </sst>
 </file>
@@ -2390,10 +2411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE263883-2701-4B73-BA24-C20413007C34}">
-  <dimension ref="B2:F241"/>
+  <dimension ref="B2:F244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="E247" sqref="E247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6442,6 +6463,42 @@
         <v>123</v>
       </c>
     </row>
+    <row r="242" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <v>3000</v>
+      </c>
+      <c r="C242" t="s">
+        <v>660</v>
+      </c>
+      <c r="D242" t="s">
+        <v>661</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="243" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <v>4000</v>
+      </c>
+      <c r="C243" t="s">
+        <v>664</v>
+      </c>
+      <c r="D243" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="244" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <v>5000</v>
+      </c>
+      <c r="C244" t="s">
+        <v>665</v>
+      </c>
+      <c r="D244" t="s">
+        <v>666</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Intégration d'un framework d'équilibrage des stats des armes
</commit_message>
<xml_diff>
--- a/Documentation/Items.xlsx
+++ b/Documentation/Items.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity_Projects\LC_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DB1C33-6E05-48F5-B15D-630C6D8AF942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43294A7D-19DA-4A97-938B-D930A1E07AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="ListOfItems" sheetId="1" r:id="rId1"/>
+    <sheet name="PowerRuling" sheetId="3" r:id="rId2"/>
+    <sheet name="Swords" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="714">
   <si>
     <t>ID</t>
   </si>
@@ -2037,6 +2039,147 @@
   </si>
   <si>
     <t>Key Item</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Mana</t>
+  </si>
+  <si>
+    <t>Essence</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>Magic</t>
+  </si>
+  <si>
+    <t>Magic Defense</t>
+  </si>
+  <si>
+    <t>Agility</t>
+  </si>
+  <si>
+    <t>Luck</t>
+  </si>
+  <si>
+    <t>Each weapon has a calculated power value, which is based on the stats and effects it gives. Rank provides a decent indication of how powerful a weapon is.</t>
+  </si>
+  <si>
+    <t>Each stat, besides HP, Mana and Essence gives 1 power for 1 point. HP gives 1 power per 10 HP, Mana 1 power per 5 MP and Essence 1 power per 5 EP</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Inflicting status also raises the power. The following negative status inflicted have the indicated power :</t>
+  </si>
+  <si>
+    <t>Bleed I</t>
+  </si>
+  <si>
+    <t>Bleed II</t>
+  </si>
+  <si>
+    <t>Bleed III</t>
+  </si>
+  <si>
+    <t>Hemo I</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>Blind</t>
+  </si>
+  <si>
+    <t>Silence</t>
+  </si>
+  <si>
+    <t>Break I</t>
+  </si>
+  <si>
+    <t>Break II</t>
+  </si>
+  <si>
+    <t>Break III</t>
+  </si>
+  <si>
+    <t>Magic Break I</t>
+  </si>
+  <si>
+    <t>Magic Break II</t>
+  </si>
+  <si>
+    <t>Magic Break III</t>
+  </si>
+  <si>
+    <t>The following bound abilities add power :</t>
+  </si>
+  <si>
+    <t>Drain Slash</t>
+  </si>
+  <si>
+    <t>Weak Point</t>
+  </si>
+  <si>
+    <t>Slow I</t>
+  </si>
+  <si>
+    <t>Slow II</t>
+  </si>
+  <si>
+    <t>Slow III</t>
+  </si>
+  <si>
+    <t>Knight's Vow</t>
+  </si>
+  <si>
+    <t>Magical Impact</t>
+  </si>
+  <si>
+    <t>Immunity</t>
+  </si>
+  <si>
+    <t>MP cost reduction is 5 power per 10%</t>
+  </si>
+  <si>
+    <t>Removes</t>
+  </si>
+  <si>
+    <t>Shell</t>
+  </si>
+  <si>
+    <t>Protect</t>
+  </si>
+  <si>
+    <t>Weapon is 2-handed (-3 * rank)</t>
+  </si>
+  <si>
+    <t>Abode of Souls</t>
+  </si>
+  <si>
+    <t>Trance</t>
+  </si>
+  <si>
+    <t>Crystal Guard</t>
+  </si>
+  <si>
+    <t>Evasive Dance</t>
+  </si>
+  <si>
+    <t>Suffers from</t>
+  </si>
+  <si>
+    <t>Holy Wrath</t>
+  </si>
+  <si>
+    <t>Rank XII, Louga's ultimate weapon.</t>
   </si>
 </sst>
 </file>
@@ -2413,8 +2556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE263883-2701-4B73-BA24-C20413007C34}">
   <dimension ref="B2:F244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="E247" sqref="E247"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6502,4 +6645,1758 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B5F246-E8D7-402E-9A8B-F3ABB3622514}">
+  <dimension ref="B2:G32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>680</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>681</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>682</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>683</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>684</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>685</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>684</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>686</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>685</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>687</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>686</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>688</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>689</v>
+      </c>
+      <c r="C15">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>690</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>704</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>691</v>
+      </c>
+      <c r="C17">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>705</v>
+      </c>
+      <c r="G17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>692</v>
+      </c>
+      <c r="C18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>696</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>697</v>
+      </c>
+      <c r="C20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>698</v>
+      </c>
+      <c r="C21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>693</v>
+      </c>
+      <c r="F23" t="s">
+        <v>682</v>
+      </c>
+      <c r="G23">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>694</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>695</v>
+      </c>
+      <c r="C25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>699</v>
+      </c>
+      <c r="C26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>700</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>707</v>
+      </c>
+      <c r="C28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>708</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>709</v>
+      </c>
+      <c r="C30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>710</v>
+      </c>
+      <c r="C31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>712</v>
+      </c>
+      <c r="C32">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFDFD57-C829-46C4-A7CF-3734419064E7}">
+  <dimension ref="B1:O33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>(F2/10)+G2/5+H2/5+I2+J2+K2+L2+M2+N2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1001</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>(F3/10)+G3/5+H3/5+I3+J3+K3+L3+M3+N3+PowerRuling!C6</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1002</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>(F4/10)+G4/5+H4/5+I4+J4+K4+L4+M4+N4</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1003</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>6</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>(F5/10)+G5/5+H5/5+I5+J5+K5+L5+M5+N5</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1004</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>(F6/10)+G6/5+H6/5+I6+J6+K6+L6+M6+N6+PowerRuling!C6+PowerRuling!C24</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1005</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>18</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>9</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>(F7/10)+G7/5+H7/5+I7+J7+K7+L7+M7+N7</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1006</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>(F8/10)+G8/5+H8/5+I8+J8+K8+L8+M8+N8+PowerRuling!C9</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1007</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>21</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>(F9/10)+G9/5+H9/5+I9+J9+K9+L9+M9+N3+3*8</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1008</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>18</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>6</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>(F10/10)+G10/5+H10/5+I10+J10+K10+L10+M10+N10+PowerRuling!C9+PowerRuling!C24+PowerRuling!C6</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1009</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>80</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>25</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>10</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>(F11/10)+G11/5+H11/5+I11+J11+K11+L11+M11+N11</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1010</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>336</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>24</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>7</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>F12+G12+H12+I12+J12+K12+L12+M12+N12+PowerRuling!C25+3*8</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1011</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13">
+        <v>80</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>28</v>
+      </c>
+      <c r="J13">
+        <v>9</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>9</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>F13/10+G13/5+H13/5+I13+J13+K13+L13+M13+N13+PowerRuling!C6+PowerRuling!C9+PowerRuling!C24</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1012</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>20</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>18</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>21</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>F14/10+G14/5+H14/5+I14+J14+K14+L14+M14+N14+PowerRuling!C16</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1013</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>28</v>
+      </c>
+      <c r="J15">
+        <v>6</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>6</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>F15/10+G15/5+H15/5+I15+J15+K15+L15+M15+N15+PowerRuling!C6+PowerRuling!C9+PowerRuling!C19+PowerRuling!C24</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1014</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16">
+        <v>120</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>34</v>
+      </c>
+      <c r="J16">
+        <v>16</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>16</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>F16/10+G16/5+H16/5+I16+J16+K16+L16+M16+N16+PowerRuling!C26</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1015</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>31</v>
+      </c>
+      <c r="J17">
+        <v>10</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>9</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>F17/10+G17/5+H17/5+I17+J17+K17+L17+M17+N17+4*8+PowerRuling!C25</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1016</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18">
+        <v>80</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>38</v>
+      </c>
+      <c r="J18">
+        <v>10</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>10</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>F18/5+G18/5+H18/5+I18+J18+K18+L18+M18+N18+PowerRuling!C6+PowerRuling!C9+PowerRuling!C10+PowerRuling!C11+PowerRuling!C19+PowerRuling!C24</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1017</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>35</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>28</v>
+      </c>
+      <c r="J19">
+        <v>15</v>
+      </c>
+      <c r="K19">
+        <v>32</v>
+      </c>
+      <c r="L19">
+        <v>15</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f>F19/10+G19/5+H19/5+I19+J19+K19+L19+M19+N19+PowerRuling!C16+PowerRuling!C27</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1018</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20">
+        <v>60</v>
+      </c>
+      <c r="G20">
+        <v>20</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>32</v>
+      </c>
+      <c r="J20">
+        <v>14</v>
+      </c>
+      <c r="K20">
+        <v>12</v>
+      </c>
+      <c r="L20">
+        <v>14</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>7</v>
+      </c>
+      <c r="O20">
+        <f>F20/10+G20/5+H20/5+I20+J20+K20+L20+M20+N20+5*4</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1019</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+      <c r="G21">
+        <v>60</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>12</v>
+      </c>
+      <c r="J21">
+        <v>14</v>
+      </c>
+      <c r="K21">
+        <v>32</v>
+      </c>
+      <c r="L21">
+        <v>14</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>7</v>
+      </c>
+      <c r="O21">
+        <f>F21/10+G21/5+H21/5+I21+J21+K21+L21+M21+N21+PowerRuling!G12+PowerRuling!G13</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1020</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22">
+        <v>200</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>42</v>
+      </c>
+      <c r="J22">
+        <v>28</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>28</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>F22/10+G22/5+H22/5+I22+J22+K22+L22+M22+N22+PowerRuling!C26</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1021</v>
+      </c>
+      <c r="C23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23">
+        <v>100</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>50</v>
+      </c>
+      <c r="J23">
+        <v>10</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>10</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>F23/10+G23/5+H23/5+I23+J23+K23+L23+M23+N23+PowerRuling!C6+PowerRuling!C9+PowerRuling!C10+PowerRuling!C11+PowerRuling!C19+PowerRuling!C13+PowerRuling!C16+PowerRuling!C24</f>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1022</v>
+      </c>
+      <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24">
+        <v>140</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>41</v>
+      </c>
+      <c r="J24">
+        <v>13</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>13</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f>F24/10+G24/5+H24/5+I24+J24+K24+L24+M24+N24+PowerRuling!C6+PowerRuling!C9+PowerRuling!C10+PowerRuling!C11+PowerRuling!C19+PowerRuling!C24+PowerRuling!G16+PowerRuling!G17</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1023</v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25">
+        <v>300</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>54</v>
+      </c>
+      <c r="J25">
+        <v>42</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>42</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f>F25/10+G25/5+H25/5+I25+J25+K25+L25+M25+N25+-3*10+PowerRuling!C26</f>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1024</v>
+      </c>
+      <c r="C26" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>51</v>
+      </c>
+      <c r="J26">
+        <v>18</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>18</v>
+      </c>
+      <c r="M26">
+        <v>15</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f>F26/10+G26/5+H26/5+I26+J26+K26+L26+M26+N26+5*8+PowerRuling!C25</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1025</v>
+      </c>
+      <c r="C27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27">
+        <v>60</v>
+      </c>
+      <c r="G27">
+        <v>20</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>25</v>
+      </c>
+      <c r="J27">
+        <v>14</v>
+      </c>
+      <c r="K27">
+        <v>25</v>
+      </c>
+      <c r="L27">
+        <v>14</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>7</v>
+      </c>
+      <c r="O27">
+        <f>F27/10+G27/5+H27/5+I27+J27+K27+L27+M27+N27+5*4+PowerRuling!G12+PowerRuling!G13+PowerRuling!C28</f>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>1026</v>
+      </c>
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>60</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>40</v>
+      </c>
+      <c r="J28">
+        <v>18</v>
+      </c>
+      <c r="K28">
+        <v>55</v>
+      </c>
+      <c r="L28">
+        <v>26</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f>F28/10+G28/5+H28/5+I28+J28+K28+L28+M28+N28+PowerRuling!C16+PowerRuling!C27+PowerRuling!C29</f>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>1027</v>
+      </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29">
+        <v>250</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>42</v>
+      </c>
+      <c r="J29">
+        <v>40</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>40</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f>F29/10+G29/5+H29/5+I29+J29+K29+L29+M29+N29+PowerRuling!C26+PowerRuling!C30</f>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>1028</v>
+      </c>
+      <c r="C30" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>60</v>
+      </c>
+      <c r="J30">
+        <v>18</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>18</v>
+      </c>
+      <c r="M30">
+        <v>15</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f>F30/10+G30/5+H30/5+I30+J30+K30+L30+M30+N30+5*8+PowerRuling!C25+PowerRuling!C31</f>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>1029</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E31" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31">
+        <v>150</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>100</v>
+      </c>
+      <c r="J31">
+        <v>35</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>35</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f>F31/10+G31/5+H31/5+I31+J31+K31+L31+M31+N31+PowerRuling!C6+PowerRuling!C9+PowerRuling!C10+PowerRuling!C11+PowerRuling!C19+PowerRuling!C24+PowerRuling!G23</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1030</v>
+      </c>
+      <c r="C32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>60</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>45</v>
+      </c>
+      <c r="J32">
+        <v>18</v>
+      </c>
+      <c r="K32">
+        <v>60</v>
+      </c>
+      <c r="L32">
+        <v>26</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f>F32/10+G32/5+H32/5+I32+J32+K32+L32+M32+N32+PowerRuling!C16+PowerRuling!C27+PowerRuling!C29+PowerRuling!C32</f>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1031</v>
+      </c>
+      <c r="C33" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" t="s">
+        <v>713</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Les épées et les dagues sont dans le framework
</commit_message>
<xml_diff>
--- a/Documentation/Items.xlsx
+++ b/Documentation/Items.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity_Projects\LC_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43294A7D-19DA-4A97-938B-D930A1E07AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CE9C26-457C-4273-85B9-1BA57F173E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
   </bookViews>
   <sheets>
     <sheet name="ListOfItems" sheetId="1" r:id="rId1"/>
     <sheet name="PowerRuling" sheetId="3" r:id="rId2"/>
     <sheet name="Swords" sheetId="2" r:id="rId3"/>
+    <sheet name="Daggers" sheetId="4" r:id="rId4"/>
+    <sheet name="Axes" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="724">
   <si>
     <t>ID</t>
   </si>
@@ -2180,6 +2182,36 @@
   </si>
   <si>
     <t>Rank XII, Louga's ultimate weapon.</t>
+  </si>
+  <si>
+    <t>Effectiveness of potions</t>
+  </si>
+  <si>
+    <t>Sinister Strike</t>
+  </si>
+  <si>
+    <t>Deals bonus dmg against type</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>strong</t>
+  </si>
+  <si>
+    <t>First Aid</t>
+  </si>
+  <si>
+    <t>Camouflage</t>
+  </si>
+  <si>
+    <t>Elemental affinity dmg reduction (1 per 10% per element)</t>
+  </si>
+  <si>
+    <t>Bloody Murder</t>
+  </si>
+  <si>
+    <t>Curative Fog</t>
   </si>
 </sst>
 </file>
@@ -2556,8 +2588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE263883-2701-4B73-BA24-C20413007C34}">
   <dimension ref="B2:F244"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:F45"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46:F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6649,34 +6681,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B5F246-E8D7-402E-9A8B-F3ABB3622514}">
-  <dimension ref="B2:G32"/>
+  <dimension ref="B2:L37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>680</v>
       </c>
@@ -6684,7 +6717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>681</v>
       </c>
@@ -6692,7 +6725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>682</v>
       </c>
@@ -6702,8 +6735,14 @@
       <c r="F8" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>714</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>683</v>
       </c>
@@ -6711,7 +6750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>684</v>
       </c>
@@ -6721,8 +6760,11 @@
       <c r="F10" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>685</v>
       </c>
@@ -6735,8 +6777,14 @@
       <c r="G11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>717</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>686</v>
       </c>
@@ -6749,8 +6797,14 @@
       <c r="G12">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>718</v>
+      </c>
+      <c r="L12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>687</v>
       </c>
@@ -6764,7 +6818,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>688</v>
       </c>
@@ -6772,7 +6826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>689</v>
       </c>
@@ -6783,7 +6837,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>690</v>
       </c>
@@ -6885,6 +6939,9 @@
       <c r="C26">
         <v>13</v>
       </c>
+      <c r="F26" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
@@ -6932,6 +6989,46 @@
       </c>
       <c r="C32">
         <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>715</v>
+      </c>
+      <c r="C33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>719</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>720</v>
+      </c>
+      <c r="C35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>722</v>
+      </c>
+      <c r="C36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>723</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -6943,8 +7040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFDFD57-C829-46C4-A7CF-3734419064E7}">
   <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8399,4 +8496,985 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A67A6C-BD76-4F63-B522-FA55F75B46B2}">
+  <dimension ref="B1:O22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1032</v>
+      </c>
+      <c r="C2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>5</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>F2/10+G2/5+H2/5+I2+J2+K2+L2+M2+N2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1033</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1034</v>
+      </c>
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>F4/10+G4/5+H4/5+I4+J4+K4+L4+M4+N4+PowerRuling!L8</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1035</v>
+      </c>
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>F5/10+G5/5+H5/5+I5+J5+K5+L5+M5+N5+PowerRuling!C10</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1036</v>
+      </c>
+      <c r="C6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>9</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>8</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>F6/10+G6/5+H6/5+I6+J6+K6+L6+M6+N6+1*8</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1037</v>
+      </c>
+      <c r="C7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>7</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>F7/10+G7/5+H7/5+I7+J7+K7+L7+M7+N7+PowerRuling!C10+PowerRuling!C33</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1038</v>
+      </c>
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>9</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>F8/10+G8/5+H8/5+I8+J8+K8+L8+M8+N8+1*8+PowerRuling!L11</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1039</v>
+      </c>
+      <c r="C9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>13</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>F9/10+G9/5+H9/5+I9+J9+K9+L9+M9+N9+PowerRuling!L8+PowerRuling!C34</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1040</v>
+      </c>
+      <c r="C10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>19</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>18</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>F10/10+G10/5+H10/5+I10+J10+K10+L10+M10+N10+1*8+PowerRuling!L11</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1041</v>
+      </c>
+      <c r="C11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>26</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>26</v>
+      </c>
+      <c r="N11">
+        <v>6</v>
+      </c>
+      <c r="O11">
+        <f>F11/10+G11/5+H11/5+I11+J11+K11+L11+M11+N11+1*8+PowerRuling!L11</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1042</v>
+      </c>
+      <c r="C12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" t="s">
+        <v>154</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>19</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>26</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>F12/10+G12/5+H12/5+I12+J12+K12+L12+M12+N12+PowerRuling!C10+PowerRuling!C11+1*8+PowerRuling!C33</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1043</v>
+      </c>
+      <c r="C13" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>11</v>
+      </c>
+      <c r="J13">
+        <v>14</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>28</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>F13/10+G13/5+H13/5+I13+J13+K13+L13+M13+N13+1*8+PowerRuling!C34+PowerRuling!L8</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1044</v>
+      </c>
+      <c r="C14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E14" t="s">
+        <v>159</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>28</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>52</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>F14/10+G14/5+H14/5+I14+J14+K14+L14+M14+N14+PowerRuling!C6+PowerRuling!C9</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1045</v>
+      </c>
+      <c r="C15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>32</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>32</v>
+      </c>
+      <c r="N15">
+        <v>12</v>
+      </c>
+      <c r="O15">
+        <f>F15/10+G15/5+H15/5+I15+J15+K15+L15+M15+N15+PowerRuling!C35+PowerRuling!L12</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1046</v>
+      </c>
+      <c r="C16" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>44</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>70</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>F16/10+G16/5+H16/5+I16+J16+K16+L16+M16+N16+PowerRuling!C6+PowerRuling!C9+5*1</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1047</v>
+      </c>
+      <c r="C17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E17" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>44</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>48</v>
+      </c>
+      <c r="N17">
+        <v>15</v>
+      </c>
+      <c r="O17">
+        <f>F17/10+G17/5+H17/5+I17+J17+K17+L17+M17+N17+1*8+PowerRuling!C35+PowerRuling!L12</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1048</v>
+      </c>
+      <c r="C18" t="s">
+        <v>179</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E18" t="s">
+        <v>168</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>50</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>85</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>F18/10+G18/5+H18/5+I18+J18+K18+L18+M18+N18+PowerRuling!C6+PowerRuling!C9+PowerRuling!L11</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1049</v>
+      </c>
+      <c r="C19" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E19" t="s">
+        <v>169</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>40</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>70</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f>F19/10+G19/5+H19/5+I19+J19+K19+L19+M19+N19+PowerRuling!C10+PowerRuling!C11+PowerRuling!C12+1*8+PowerRuling!C33+PowerRuling!C36</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1050</v>
+      </c>
+      <c r="C20" t="s">
+        <v>183</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>23</v>
+      </c>
+      <c r="J20">
+        <v>55</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>60</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f>F20/10+G20/5+H20/5+I20+J20+K20+L20+M20+N20+PowerRuling!L8+2*8+PowerRuling!C34+PowerRuling!C37</f>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1051</v>
+      </c>
+      <c r="C21" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>60</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>90</v>
+      </c>
+      <c r="N21">
+        <v>28</v>
+      </c>
+      <c r="O21">
+        <f>F21/10+G21/5+H21/5+I21+J21+K21+L21+M21+N21+PowerRuling!C35+PowerRuling!L12+1*8</f>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1052</v>
+      </c>
+      <c r="C22" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71C5CED-70F3-4061-8153-EB3DDD81F3FA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Haches intégrées au framework
</commit_message>
<xml_diff>
--- a/Documentation/Items.xlsx
+++ b/Documentation/Items.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity_Projects\LC_Unity\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxad\Documents\git_projects\LC_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CE9C26-457C-4273-85B9-1BA57F173E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3959A23-E8E7-4869-9CD4-EA4429528489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="732">
   <si>
     <t>ID</t>
   </si>
@@ -2212,6 +2212,30 @@
   </si>
   <si>
     <t>Curative Fog</t>
+  </si>
+  <si>
+    <t>Axe Throw</t>
+  </si>
+  <si>
+    <t>Cleave</t>
+  </si>
+  <si>
+    <t>Crush</t>
+  </si>
+  <si>
+    <t>Grounded</t>
+  </si>
+  <si>
+    <t>Lifedrain</t>
+  </si>
+  <si>
+    <t>Bloodbath</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>Endless Rampage</t>
   </si>
 </sst>
 </file>
@@ -2588,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE263883-2701-4B73-BA24-C20413007C34}">
   <dimension ref="B2:F244"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46:F66"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67:F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6681,10 +6705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B5F246-E8D7-402E-9A8B-F3ABB3622514}">
-  <dimension ref="B2:L37"/>
+  <dimension ref="B2:L43"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6825,6 +6849,12 @@
       <c r="C14">
         <v>14</v>
       </c>
+      <c r="K14" t="s">
+        <v>728</v>
+      </c>
+      <c r="L14">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -6901,6 +6931,12 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>727</v>
+      </c>
+      <c r="C22">
+        <v>14</v>
+      </c>
       <c r="F22" t="s">
         <v>711</v>
       </c>
@@ -7029,6 +7065,54 @@
       </c>
       <c r="C37">
         <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>724</v>
+      </c>
+      <c r="C38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>725</v>
+      </c>
+      <c r="C39">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>726</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>729</v>
+      </c>
+      <c r="C41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>730</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>731</v>
+      </c>
+      <c r="C43">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -7040,7 +7124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFDFD57-C829-46C4-A7CF-3734419064E7}">
   <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
@@ -8502,8 +8586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A67A6C-BD76-4F63-B522-FA55F75B46B2}">
   <dimension ref="B1:O22"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9467,14 +9551,835 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71C5CED-70F3-4061-8153-EB3DDD81F3FA}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1053</v>
+      </c>
+      <c r="C2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>F2/10+G2/5+H2+I2+J2+K2+L2+M2+N2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1054</v>
+      </c>
+      <c r="C3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" t="s">
+        <v>205</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O19" si="0">F3/10+G3/5+H3+I3+J3+K3+L3+M3+N3</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1055</v>
+      </c>
+      <c r="C4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F4">
+        <v>70</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>18</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="120" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1056</v>
+      </c>
+      <c r="C5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5">
+        <v>80</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>21</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>F5/10+G5/5+H5+I5+J5+K5+L5+M5+N5+PowerRuling!C6</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1057</v>
+      </c>
+      <c r="C6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" t="s">
+        <v>209</v>
+      </c>
+      <c r="F6">
+        <v>70</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>F6/10+G6/5+H6+I6+J6+K6+L6+M6+N6+PowerRuling!C19</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1058</v>
+      </c>
+      <c r="C7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" t="s">
+        <v>211</v>
+      </c>
+      <c r="F7">
+        <v>80</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>26</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>F7/10+G7/5+H7+I7+J7+K7+L7+M7+N7+1*8</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="195" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1059</v>
+      </c>
+      <c r="C8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8">
+        <v>90</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>28</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>F8/10+G8/5+H8+I8+J8+K8+L8+M8+N8+PowerRuling!C6+1*8</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1060</v>
+      </c>
+      <c r="C9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F9">
+        <v>110</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>34</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>F9/10+G9/5+H9+I9+J9+K9+L9+M9+N9+PowerRuling!C19+PowerRuling!C9</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1061</v>
+      </c>
+      <c r="C10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E10" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10">
+        <v>150</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>43</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>7</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>F10/10+G10/5+H10+I10+J10+K10+L10+M10+N10+PowerRuling!C6+PowerRuling!C38</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1062</v>
+      </c>
+      <c r="C11" t="s">
+        <v>195</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E11" t="s">
+        <v>219</v>
+      </c>
+      <c r="F11">
+        <v>240</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>40</v>
+      </c>
+      <c r="J11">
+        <v>16</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>16</v>
+      </c>
+      <c r="M11">
+        <v>-10</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>F11/10+G11/5+H11+I11+J11+K11+L11+M11+N11+1*8+PowerRuling!C6+PowerRuling!C39</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1063</v>
+      </c>
+      <c r="C12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E12" t="s">
+        <v>221</v>
+      </c>
+      <c r="F12">
+        <v>80</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>55</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>16</v>
+      </c>
+      <c r="M12">
+        <v>-10</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>F12/10+G12/5+H12+I12+J12+K12+L12+M12+N12+1*8+PowerRuling!C40</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1064</v>
+      </c>
+      <c r="C13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13">
+        <v>200</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>48</v>
+      </c>
+      <c r="J13">
+        <v>14</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>14</v>
+      </c>
+      <c r="M13">
+        <v>-10</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>F13/10+G13/5+H13+I13+J13+K13+L13+M13+N13+PowerRuling!C41+PowerRuling!L14</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1065</v>
+      </c>
+      <c r="C14" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F14">
+        <v>200</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>49</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>20</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>F14/10+G14/5+H14+I14+J14+K14+L14+M14+N14+PowerRuling!C6+PowerRuling!C38+2*8</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1066</v>
+      </c>
+      <c r="C15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E15" t="s">
+        <v>226</v>
+      </c>
+      <c r="F15">
+        <v>200</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>55</v>
+      </c>
+      <c r="J15">
+        <v>15</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>15</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>F15/10+G15/5+H15+I15+J15+K15+L15+M15+N15+PowerRuling!C9+PowerRuling!C19+PowerRuling!C42</f>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1067</v>
+      </c>
+      <c r="C16" t="s">
+        <v>201</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E16" t="s">
+        <v>228</v>
+      </c>
+      <c r="F16">
+        <v>200</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>49</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>24</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>F16/10+G16/5+H16+I16+J16+K16+L16+M16+N16+PowerRuling!C6+2*8+PowerRuling!C38+PowerRuling!C43</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1068</v>
+      </c>
+      <c r="C17" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E17" t="s">
+        <v>232</v>
+      </c>
+      <c r="F17">
+        <v>300</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>65</v>
+      </c>
+      <c r="J17">
+        <v>20</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>20</v>
+      </c>
+      <c r="M17">
+        <v>-10</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>F17/10+G17/5+H17+I17+J17+K17+L17+M17+N17+2*8+PowerRuling!C6+PowerRuling!C39+PowerRuling!C40</f>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1069</v>
+      </c>
+      <c r="C18" t="s">
+        <v>203</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E18" t="s">
+        <v>234</v>
+      </c>
+      <c r="F18">
+        <v>200</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>80</v>
+      </c>
+      <c r="J18">
+        <v>18</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>18</v>
+      </c>
+      <c r="M18">
+        <v>-10</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>F18/10+G18/5+H18+I18+J18+K18+L18+M18+N18+1*8+PowerRuling!L14+PowerRuling!C40+PowerRuling!C41</f>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1070</v>
+      </c>
+      <c r="C19" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E19" t="s">
+        <v>229</v>
+      </c>
+      <c r="O19">
+        <f>F19/10+G19/5+H19+I19+J19+K19+L19+M19+N19</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Griffes, sceptres, bâtons, grimoires
</commit_message>
<xml_diff>
--- a/Documentation/Items.xlsx
+++ b/Documentation/Items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxad\Documents\git_projects\LC_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3959A23-E8E7-4869-9CD4-EA4429528489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC25F690-48ED-42D2-8758-9845A822E7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
   </bookViews>
   <sheets>
     <sheet name="ListOfItems" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="Swords" sheetId="2" r:id="rId3"/>
     <sheet name="Daggers" sheetId="4" r:id="rId4"/>
     <sheet name="Axes" sheetId="5" r:id="rId5"/>
+    <sheet name="Claws" sheetId="6" r:id="rId6"/>
+    <sheet name="Scepters" sheetId="7" r:id="rId7"/>
+    <sheet name="Staves" sheetId="8" r:id="rId8"/>
+    <sheet name="Grimoire" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="752">
   <si>
     <t>ID</t>
   </si>
@@ -2160,9 +2164,6 @@
     <t>Protect</t>
   </si>
   <si>
-    <t>Weapon is 2-handed (-3 * rank)</t>
-  </si>
-  <si>
     <t>Abode of Souls</t>
   </si>
   <si>
@@ -2236,6 +2237,69 @@
   </si>
   <si>
     <t>Endless Rampage</t>
+  </si>
+  <si>
+    <t>Claws malus per rank</t>
+  </si>
+  <si>
+    <t>Howling Moon</t>
+  </si>
+  <si>
+    <t>Claw Storm</t>
+  </si>
+  <si>
+    <t>Weapon is 2-handed (per rank)</t>
+  </si>
+  <si>
+    <t>Crystal Breach</t>
+  </si>
+  <si>
+    <t>Elemental dmg increase (1 per 10%)</t>
+  </si>
+  <si>
+    <t>Essence Boost</t>
+  </si>
+  <si>
+    <t>Hand of Protection</t>
+  </si>
+  <si>
+    <t>Essence Flux</t>
+  </si>
+  <si>
+    <t>Saving Light</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Negate</t>
+  </si>
+  <si>
+    <t>Void Beam</t>
+  </si>
+  <si>
+    <t>Magic Counter</t>
+  </si>
+  <si>
+    <t>Jouvence</t>
+  </si>
+  <si>
+    <t>Wisdom</t>
+  </si>
+  <si>
+    <t>Mana Well</t>
+  </si>
+  <si>
+    <t>Pain Blast</t>
+  </si>
+  <si>
+    <t>Purify</t>
+  </si>
+  <si>
+    <t>Flare</t>
+  </si>
+  <si>
+    <t>Doom</t>
   </si>
 </sst>
 </file>
@@ -2612,8 +2676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE263883-2701-4B73-BA24-C20413007C34}">
   <dimension ref="B2:F244"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67:F84"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6705,16 +6769,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B5F246-E8D7-402E-9A8B-F3ABB3622514}">
-  <dimension ref="B2:L43"/>
+  <dimension ref="B2:L60"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" customWidth="1"/>
     <col min="11" max="11" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6760,7 +6824,7 @@
         <v>702</v>
       </c>
       <c r="K8" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="L8">
         <v>5</v>
@@ -6785,7 +6849,7 @@
         <v>701</v>
       </c>
       <c r="K10" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -6802,7 +6866,7 @@
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="L11">
         <v>4</v>
@@ -6822,7 +6886,7 @@
         <v>8</v>
       </c>
       <c r="K12" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="L12">
         <v>6</v>
@@ -6849,8 +6913,14 @@
       <c r="C14">
         <v>14</v>
       </c>
+      <c r="F14" t="s">
+        <v>741</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
       <c r="K14" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="L14">
         <v>10</v>
@@ -6911,7 +6981,10 @@
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>706</v>
+        <v>734</v>
+      </c>
+      <c r="G19">
+        <v>-3</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -6932,13 +7005,13 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C22">
         <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -6976,7 +7049,7 @@
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -6986,10 +7059,13 @@
       <c r="C27">
         <v>6</v>
       </c>
+      <c r="F27" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="C28">
         <v>18</v>
@@ -6997,15 +7073,21 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="C29">
         <v>8</v>
       </c>
+      <c r="F29" t="s">
+        <v>731</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C30">
         <v>15</v>
@@ -7013,7 +7095,7 @@
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C31">
         <v>15</v>
@@ -7021,7 +7103,7 @@
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C32">
         <v>22</v>
@@ -7029,7 +7111,7 @@
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C33">
         <v>7</v>
@@ -7037,7 +7119,7 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C34">
         <v>6</v>
@@ -7045,7 +7127,7 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C35">
         <v>9</v>
@@ -7053,7 +7135,7 @@
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C36">
         <v>9</v>
@@ -7061,7 +7143,7 @@
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C37">
         <v>10</v>
@@ -7069,7 +7151,7 @@
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C38">
         <v>20</v>
@@ -7077,7 +7159,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C39">
         <v>11</v>
@@ -7085,7 +7167,7 @@
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C40">
         <v>16</v>
@@ -7093,7 +7175,7 @@
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C41">
         <v>14</v>
@@ -7101,7 +7183,7 @@
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C42">
         <v>10</v>
@@ -7109,10 +7191,146 @@
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C43">
         <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>732</v>
+      </c>
+      <c r="C44">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>733</v>
+      </c>
+      <c r="C45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>735</v>
+      </c>
+      <c r="C46">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>737</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>738</v>
+      </c>
+      <c r="C48">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>739</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>740</v>
+      </c>
+      <c r="C50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>742</v>
+      </c>
+      <c r="C51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>743</v>
+      </c>
+      <c r="C52">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>744</v>
+      </c>
+      <c r="C53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>745</v>
+      </c>
+      <c r="C54">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>746</v>
+      </c>
+      <c r="C55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>747</v>
+      </c>
+      <c r="C56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>748</v>
+      </c>
+      <c r="C57">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>749</v>
+      </c>
+      <c r="C58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>750</v>
+      </c>
+      <c r="C59">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>751</v>
+      </c>
+      <c r="C60">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -7124,8 +7342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFDFD57-C829-46C4-A7CF-3734419064E7}">
   <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8244,7 +8462,7 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <f>F25/10+G25/5+H25/5+I25+J25+K25+L25+M25+N25+-3*10+PowerRuling!C26</f>
+        <f>F25/10+G25/5+H25/5+I25+J25+K25+L25+M25+N25+PowerRuling!G19*10+PowerRuling!C26</f>
         <v>151</v>
       </c>
     </row>
@@ -8574,7 +8792,7 @@
         <v>113</v>
       </c>
       <c r="E33" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
   </sheetData>
@@ -9553,7 +9771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71C5CED-70F3-4061-8153-EB3DDD81F3FA}">
   <dimension ref="B1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -9682,7 +9900,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O19" si="0">F3/10+G3/5+H3+I3+J3+K3+L3+M3+N3</f>
+        <f t="shared" ref="O3:O4" si="0">F3/10+G3/5+H3+I3+J3+K3+L3+M3+N3</f>
         <v>15</v>
       </c>
     </row>
@@ -10377,6 +10595,3098 @@
       <c r="O19">
         <f>F19/10+G19/5+H19+I19+J19+K19+L19+M19+N19</f>
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52245DA4-B6A7-43F4-9E25-B651EFDB9442}">
+  <dimension ref="B1:O15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1071</v>
+      </c>
+      <c r="C2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>6</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>F2/10+G2/5+H2/5+I2+J2+K2+L2+M2+N2+PowerRuling!$G$29*3</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1072</v>
+      </c>
+      <c r="C3" t="s">
+        <v>237</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3+PowerRuling!$G$29*4</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1073</v>
+      </c>
+      <c r="C4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>13</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>6</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>F4/10+G4/5+H4/5+I4+J4+K4+L4+M4+N4+PowerRuling!$G$29*5+PowerRuling!C44</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1074</v>
+      </c>
+      <c r="C5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E5" t="s">
+        <v>256</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>15</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>7</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>F5/10+G5/5+H5/5+I5+J5+K5+L5+M5+N5+PowerRuling!$G$29*5+1*8</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1075</v>
+      </c>
+      <c r="C6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>23</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>11</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>F6/10+G6/5+H6/5+I6+J6+K6+L6+M6+N6+PowerRuling!$G$29*6+1*8</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1076</v>
+      </c>
+      <c r="C7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>18</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>7</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>F7/10+G7/5+H7/5+I7+J7+K7+L7+M7+N7+PowerRuling!$G$29*6+PowerRuling!C6+PowerRuling!C12</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1077</v>
+      </c>
+      <c r="C8" t="s">
+        <v>245</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E8" t="s">
+        <v>260</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>34</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>18</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>F8/10+G8/5+H8/5+I8+J8+K8+L8+M8+N8+PowerRuling!$G$29*8+2*8</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1078</v>
+      </c>
+      <c r="C9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E9" t="s">
+        <v>262</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>28</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>31</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>F9/10+G9/5+H9/5+I9+J9+K9+L9+M9+N9+PowerRuling!$G$29*8+1*8+PowerRuling!C44</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1079</v>
+      </c>
+      <c r="C10" t="s">
+        <v>249</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E10" t="s">
+        <v>264</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>32</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>25</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>22</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>F10/10+G10/5+H10/5+I10+J10+K10+L10+M10+N10+PowerRuling!$G$29*9+PowerRuling!C6+PowerRuling!C10+PowerRuling!C12</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1080</v>
+      </c>
+      <c r="C11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E11" t="s">
+        <v>266</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>37</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>18</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>F11/10+G11/5+H11/5+I11+J11+K11+L11+M11+N11+PowerRuling!$G$29*9+2*8+PowerRuling!C45</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1081</v>
+      </c>
+      <c r="C12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E12" t="s">
+        <v>267</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>42</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>45</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>F12/10+G12/5+H12/5+I12+J12+K12+L12+M12+N12+PowerRuling!$G$29*10+1*8+PowerRuling!C44+PowerRuling!L12</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1082</v>
+      </c>
+      <c r="C13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E13" t="s">
+        <v>268</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>45</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>36</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>24</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>F13/10+G13/5+H13/5+I13+J13+K13+L13+M13+N13+PowerRuling!$G$29*11+PowerRuling!C6+PowerRuling!C10+PowerRuling!C12+PowerRuling!L12</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1083</v>
+      </c>
+      <c r="C14" t="s">
+        <v>242</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E14" t="s">
+        <v>269</v>
+      </c>
+      <c r="F14">
+        <v>250</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>50</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>34</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>F14/10+G14/5+H14/5+I14+J14+K14+L14+M14+N14+PowerRuling!$G$29*12+2*8+PowerRuling!C45+PowerRuling!C46</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1084</v>
+      </c>
+      <c r="C15" t="s">
+        <v>243</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E15" t="s">
+        <v>270</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>64</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>55</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>F15/10+G15/5+H15/5+I15+J15+K15+L15+M15+N15+PowerRuling!$G$29*12+2*8+PowerRuling!C44+PowerRuling!L12</f>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09AA25AD-0CA4-48E8-92CF-38BBD575942E}">
+  <dimension ref="B1:O24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="5" max="5" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1085</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>12</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>F2/10+G2/5+H2/5+I2+J2+K2+L2+M2+N2+PowerRuling!$G$19*2+1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1086</v>
+      </c>
+      <c r="C3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>75</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3+PowerRuling!$G$19*3+3</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1087</v>
+      </c>
+      <c r="C4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>40</v>
+      </c>
+      <c r="H4">
+        <v>25</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>9</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>F4/10+G4/5+H4/5+I4+J4+K4+L4+M4+N4+PowerRuling!$G$19*3+1*8</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1088</v>
+      </c>
+      <c r="C5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="E5" t="s">
+        <v>288</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>60</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>19</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>F5/10+G5/5+H5/5+I5+J5+K5+L5+M5+N5+PowerRuling!$G$19*4+5*2.5+1.5</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1089</v>
+      </c>
+      <c r="C6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E6" t="s">
+        <v>289</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>90</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>16</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>F6/10+G6/5+H6/5+I6+J6+K6+L6+M6+N6+PowerRuling!$G$19*4+3+2*5</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1090</v>
+      </c>
+      <c r="C7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E7" t="s">
+        <v>290</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>40</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>19</v>
+      </c>
+      <c r="L7">
+        <v>6</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>F7/10+G7/5+H7/5+I7+J7+K7+L7+M7+N7+PowerRuling!$G$19*5+1*8+PowerRuling!C47</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1091</v>
+      </c>
+      <c r="C8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E8" t="s">
+        <v>291</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>120</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="K8">
+        <v>32</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>F8/10+G8/5+H8/5+I8+J8+K8+L8+M8+N8+PowerRuling!$G$19*6+2+5*2.5+5</f>
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1092</v>
+      </c>
+      <c r="C9" t="s">
+        <v>285</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E9" t="s">
+        <v>291</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>80</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>46</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>F9/10+G9/5+H9/5+I9+J9+K9+L9+M9+N9+PowerRuling!$G$19*6+2+5*2.5+5</f>
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1093</v>
+      </c>
+      <c r="C10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E10" t="s">
+        <v>291</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>80</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>46</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>F10/10+G10/5+H10/5+I10+J10+K10+L10+M10+N10+PowerRuling!$G$19*6+2+5*2.5+5</f>
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1094</v>
+      </c>
+      <c r="C11" t="s">
+        <v>287</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E11" t="s">
+        <v>291</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>120</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>32</v>
+      </c>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>F11/10+G11/5+H11/5+I11+J11+K11+L11+M11+N11+PowerRuling!$G$19*6+2+5*2.5+5</f>
+        <v>69.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1095</v>
+      </c>
+      <c r="C12" t="s">
+        <v>282</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E12" t="s">
+        <v>292</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>150</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>31</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>F12/10+G12/5+H12/5+I12+J12+K12+L12+M12+N12+PowerRuling!$G$19*6+3+2*5+PowerRuling!C48</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1096</v>
+      </c>
+      <c r="C13" t="s">
+        <v>283</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E13" t="s">
+        <v>293</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>80</v>
+      </c>
+      <c r="H13">
+        <v>60</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>35</v>
+      </c>
+      <c r="L13">
+        <v>12</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>F13/10+G13/5+H13/5+I13+J13+K13+L13+M13+N13+PowerRuling!$G$19*7+2*8+PowerRuling!C47</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1097</v>
+      </c>
+      <c r="C14" t="s">
+        <v>294</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E14" t="s">
+        <v>299</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>180</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <v>68</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>F14/10+G14/5+H14/5+I14+J14+K14+L14+M14+N14+PowerRuling!$G$19*8+2+3.5*5+5</f>
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1098</v>
+      </c>
+      <c r="C15" t="s">
+        <v>295</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E15" t="s">
+        <v>299</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>120</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>17</v>
+      </c>
+      <c r="K15">
+        <v>52</v>
+      </c>
+      <c r="L15">
+        <v>17</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>F15/10+G15/5+H15/5+I15+J15+K15+L15+M15+N15+PowerRuling!$G$19*8+2+3.5*5+5</f>
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1099</v>
+      </c>
+      <c r="C16" t="s">
+        <v>296</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E16" t="s">
+        <v>299</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>240</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>56</v>
+      </c>
+      <c r="L16">
+        <v>3</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>F16/10+G16/5+H16/5+I16+J16+K16+L16+M16+N16+PowerRuling!$G$19*8+2+3.5*5+5</f>
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1100</v>
+      </c>
+      <c r="C17" t="s">
+        <v>297</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E17" t="s">
+        <v>299</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>140</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>76</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>F17/10+G17/5+H17/5+I17+J17+K17+L17+M17+N17+PowerRuling!$G$19*8+2+3.5*5+5</f>
+        <v>110.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1101</v>
+      </c>
+      <c r="C18" t="s">
+        <v>302</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E18" t="s">
+        <v>307</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>180</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>12</v>
+      </c>
+      <c r="K18">
+        <v>50</v>
+      </c>
+      <c r="L18">
+        <v>12</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>F18/10+G18/5+H18/5+I18+J18+K18+L18+M18+N18+PowerRuling!$G$19*9+4+5*4+PowerRuling!C48+PowerRuling!G13</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1102</v>
+      </c>
+      <c r="C19" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E19" t="s">
+        <v>308</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>120</v>
+      </c>
+      <c r="H19">
+        <v>80</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>18</v>
+      </c>
+      <c r="K19">
+        <v>50</v>
+      </c>
+      <c r="L19">
+        <v>18</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f>F19/10+G19/5+H19/5+I19+J19+K19+L19+M19+N19+PowerRuling!$G$19*9+3*8+PowerRuling!C47</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1103</v>
+      </c>
+      <c r="C20" t="s">
+        <v>305</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E20" t="s">
+        <v>309</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>120</v>
+      </c>
+      <c r="H20">
+        <v>120</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>18</v>
+      </c>
+      <c r="K20">
+        <v>54</v>
+      </c>
+      <c r="L20">
+        <v>18</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f>F20/10+G20/5+H20/5+I20+J20+K20+L20+M20+N20+PowerRuling!$G$19*10+3*8+PowerRuling!C47+PowerRuling!C49</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1104</v>
+      </c>
+      <c r="C21" t="s">
+        <v>301</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E21" t="s">
+        <v>310</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>180</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>12</v>
+      </c>
+      <c r="K21">
+        <v>56</v>
+      </c>
+      <c r="L21">
+        <v>12</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f>F21/10+G21/5+H21/5+I21+J21+K21+L21+M21+N21+PowerRuling!$G$19*10+5+5*4+PowerRuling!C48+PowerRuling!G13+PowerRuling!C50</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1105</v>
+      </c>
+      <c r="C22" t="s">
+        <v>306</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E22" t="s">
+        <v>311</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>180</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>12</v>
+      </c>
+      <c r="K22">
+        <v>62</v>
+      </c>
+      <c r="L22">
+        <v>12</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>F22/10+G22/5+H22/5+I22+J22+K22+L22+M22+N22+PowerRuling!$G$19*11+5+5*5+PowerRuling!C48+PowerRuling!C50+PowerRuling!G13+PowerRuling!G14</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1106</v>
+      </c>
+      <c r="C23" t="s">
+        <v>304</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E23" t="s">
+        <v>312</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>200</v>
+      </c>
+      <c r="H23">
+        <v>160</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>20</v>
+      </c>
+      <c r="K23">
+        <v>64</v>
+      </c>
+      <c r="L23">
+        <v>20</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>F23/10+G23/5+H23/5+I23+J23+K23+L23+M23+N23+PowerRuling!$G$19*12+3*8+PowerRuling!C49+PowerRuling!C47+20</f>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1107</v>
+      </c>
+      <c r="C24" t="s">
+        <v>298</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="E24" t="s">
+        <v>300</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>400</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>13</v>
+      </c>
+      <c r="K24">
+        <v>90</v>
+      </c>
+      <c r="L24">
+        <v>13</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f>F24/10+G24/5+H24/5+I24+J24+K24+L24+M24+N24+PowerRuling!$G$19*12+5+5*5+10</f>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77D27EC-A5E9-4AC1-8ACA-52AFB6B78A4C}">
+  <dimension ref="B1:O16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="5" max="5" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>F2/10+G2/5+H2/5+I2+J2+K2+L2+M2+N2+PowerRuling!$G$19*2</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>13</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3+PowerRuling!$G$19*2</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1110</v>
+      </c>
+      <c r="C4" t="s">
+        <v>345</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="E4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>35</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>19</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>F4/10+G4/5+H4/5+I4+J4+K4+L4+M4+N4+PowerRuling!$G$19*3</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="E5" t="s">
+        <v>353</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>35</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>18</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>F5/10+G5/5+H5/5+I5+J5+K5+L5+M5+N5+PowerRuling!$G$19*4+1*8+PowerRuling!G13</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>352</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E6" t="s">
+        <v>354</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>35</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>23</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>F6/10+G6/5+H6/5+I6+J6+K6+L6+M6+N6+PowerRuling!$G$19*4+PowerRuling!L8</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>339</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="E7" t="s">
+        <v>355</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>23</v>
+      </c>
+      <c r="L7">
+        <v>9</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>F7/10+G7/5+H7/5+I7+J7+K7+L7+M7+N7+PowerRuling!$G$19*5+3*8</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>343</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>45</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
+      </c>
+      <c r="K8">
+        <v>37</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>F8/10+G8/5+H8/5+I8+J8+K8+L8+M8+N8+PowerRuling!$G$19*5+5+PowerRuling!C51</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1115</v>
+      </c>
+      <c r="C9" t="s">
+        <v>350</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E9" t="s">
+        <v>356</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>45</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <v>40</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>F9/10+G9/5+H9/5+I9+J9+K9+L9+M9+N9+PowerRuling!$G$19*6+7.5+PowerRuling!C51+PowerRuling!C52</f>
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1116</v>
+      </c>
+      <c r="C10" t="s">
+        <v>340</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E10" t="s">
+        <v>357</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>11</v>
+      </c>
+      <c r="K10">
+        <v>34</v>
+      </c>
+      <c r="L10">
+        <v>11</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>F10/10+G10/5+H10/5+I10+J10+K10+L10+M10+N10+PowerRuling!$G$19*6+3*8+8</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>346</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E11" t="s">
+        <v>358</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>35</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>30</v>
+      </c>
+      <c r="L11">
+        <v>9</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>F11/10+G11/5+H11/5+I11+J11+K11+L11+M11+N11+PowerRuling!$G$19*7+3*8+PowerRuling!G13+PowerRuling!C21</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1118</v>
+      </c>
+      <c r="C12" t="s">
+        <v>349</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E12" t="s">
+        <v>359</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>75</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="K12">
+        <v>48</v>
+      </c>
+      <c r="L12">
+        <v>11</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>F12/10+G12/5+H12/5+I12+J12+K12+L12+M12+N12+PowerRuling!$G$19*7+1*8+PowerRuling!G13+4*2</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1119</v>
+      </c>
+      <c r="C13" t="s">
+        <v>341</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E13" t="s">
+        <v>360</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>24</v>
+      </c>
+      <c r="K13">
+        <v>70</v>
+      </c>
+      <c r="L13">
+        <v>24</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>F13/10+G13/5+H13/5+I13+J13+K13+L13+M13+N13+PowerRuling!$G$19*9+3*8+8+PowerRuling!C53</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1120</v>
+      </c>
+      <c r="C14" t="s">
+        <v>348</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="E14" t="s">
+        <v>361</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>65</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>18</v>
+      </c>
+      <c r="K14">
+        <v>70</v>
+      </c>
+      <c r="L14">
+        <v>18</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>F14/10+G14/5+H14/5+I14+J14+K14+L14+M14+N14+PowerRuling!$G$19*10+3*8+PowerRuling!G13+PowerRuling!C21+PowerRuling!L8</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1121</v>
+      </c>
+      <c r="C15" t="s">
+        <v>347</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E15" t="s">
+        <v>362</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>75</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>26</v>
+      </c>
+      <c r="K15">
+        <v>104</v>
+      </c>
+      <c r="L15">
+        <v>26</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>F15/10+G15/5+H15/5+I15+J15+K15+L15+M15+N15+PowerRuling!$G$19*11+1*8+PowerRuling!G13+4*2+6</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>342</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E16" t="s">
+        <v>363</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>32</v>
+      </c>
+      <c r="K16">
+        <v>110</v>
+      </c>
+      <c r="L16">
+        <v>32</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>F16/10+G16/5+H16/5+I16+J16+K16+L16+M16+N16+PowerRuling!$G$19*12+4*8+8+PowerRuling!C53+PowerRuling!C54</f>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584D62A5-C004-44A9-885B-19FEC1A55407}">
+  <dimension ref="B1:O13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="5" width="59" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>59</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>F2/10+G2/5+H2/5+I2+J2+L2+K2+M2+N2+PowerRuling!$G$19*5+PowerRuling!C55</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>388</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>82</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>F3/10+G3/5+H3/5+I3+J3+L3+K3+M3+N3+PowerRuling!$G$19*6+PowerRuling!C56</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>389</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>77</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>F4/10+G4/5+H4/5+I4+J4+L4+K4+M4+N4+PowerRuling!$G$19*6+PowerRuling!C57</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>390</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="E5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>99</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>F5/10+G5/5+H5/5+I5+J5+L5+K5+M5+N5+PowerRuling!$G$19*7+PowerRuling!C58</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>391</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>96</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>F6/10+G6/5+H6/5+I6+J6+L6+K6+M6+N6+PowerRuling!$G$19*7+PowerRuling!C59</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>382</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="E7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>116</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>F7/10+G7/5+H7/5+I7+J7+L7+K7+M7+N7+PowerRuling!$G$19*8+PowerRuling!C60</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1129</v>
+      </c>
+      <c r="C8" t="s">
+        <v>386</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="E8" t="s">
+        <v>392</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>136</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>F8/10+G8/5+H8/5+I8+J8+L8+K8+M8+N8+PowerRuling!$G$19*9+PowerRuling!C56+PowerRuling!C59</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1130</v>
+      </c>
+      <c r="C9" t="s">
+        <v>383</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E9" t="s">
+        <v>393</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>151</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>F9/10+G9/5+H9/5+I9+J9+L9+K9+M9+N9+PowerRuling!$G$19*10+PowerRuling!C60+PowerRuling!C57</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1131</v>
+      </c>
+      <c r="C10" t="s">
+        <v>380</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E10" t="s">
+        <v>394</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>147</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>F10/10+G10/5+H10/5+I10+J10+L10+K10+M10+N10+PowerRuling!$G$19*10+PowerRuling!C59+PowerRuling!C60</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1132</v>
+      </c>
+      <c r="C11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="E11" t="s">
+        <v>395</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>168</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>F11/10+G11/5+H11/5+I11+J11+L11+K11+M11+N11+PowerRuling!$G$19*11+PowerRuling!C56+PowerRuling!C57+PowerRuling!C60</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>385</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="E12" t="s">
+        <v>409</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>170</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>F12/10+G12/5+H12/5+I12+J12+L12+K12+M12+N12+PowerRuling!$G$19*11+PowerRuling!C58+PowerRuling!C59+PowerRuling!C56</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1134</v>
+      </c>
+      <c r="C13" t="s">
+        <v>384</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E13" t="s">
+        <v>396</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>200</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>F13/10+G13/5+H13/5+I13+J13+L13+K13+M13+N13+PowerRuling!$G$19*12+PowerRuling!C55+PowerRuling!C56+PowerRuling!C59+PowerRuling!C58</f>
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Toutes les armes sont dans le framework d'équilibrage
</commit_message>
<xml_diff>
--- a/Documentation/Items.xlsx
+++ b/Documentation/Items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxad\Documents\git_projects\LC_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506DE970-DD9A-4D58-96B1-9B07C1BCAE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833E0524-D585-4BFA-9920-9FFC57AD48AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="696" activeTab="14" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
   </bookViews>
   <sheets>
     <sheet name="ListOfItems" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,11 @@
     <sheet name="Staves" sheetId="8" r:id="rId8"/>
     <sheet name="Grimoire" sheetId="9" r:id="rId9"/>
     <sheet name="Bow" sheetId="10" r:id="rId10"/>
+    <sheet name="Arbalest" sheetId="11" r:id="rId11"/>
+    <sheet name="Spears" sheetId="12" r:id="rId12"/>
+    <sheet name="Maces" sheetId="13" r:id="rId13"/>
+    <sheet name="Firearms" sheetId="14" r:id="rId14"/>
+    <sheet name="Scythes" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="763">
   <si>
     <t>ID</t>
   </si>
@@ -2240,9 +2245,6 @@
     <t>Endless Rampage</t>
   </si>
   <si>
-    <t>Claws malus per rank</t>
-  </si>
-  <si>
     <t>Howling Moon</t>
   </si>
   <si>
@@ -2310,6 +2312,33 @@
   </si>
   <si>
     <t>Faith</t>
+  </si>
+  <si>
+    <t>Twin strike malus per rank</t>
+  </si>
+  <si>
+    <t>Bonus to shields</t>
+  </si>
+  <si>
+    <t>Counterattacks on parry</t>
+  </si>
+  <si>
+    <t>Deadly Spin</t>
+  </si>
+  <si>
+    <t>Shatter</t>
+  </si>
+  <si>
+    <t>Impair</t>
+  </si>
+  <si>
+    <t>Faster attack</t>
+  </si>
+  <si>
+    <t>Swift Strike</t>
+  </si>
+  <si>
+    <t>Attraction</t>
   </si>
 </sst>
 </file>
@@ -2686,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE263883-2701-4B73-BA24-C20413007C34}">
   <dimension ref="B2:F244"/>
   <sheetViews>
-    <sheetView topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="B149" sqref="B149:F172"/>
+    <sheetView topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="B230" sqref="B230:F238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6781,8 +6810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B29AA04-5439-44D8-B921-81D0FBC20718}">
   <dimension ref="B1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7883,12 +7912,3247 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34650302-33EE-4E55-BC98-54EF095D0F8E}">
+  <dimension ref="B1:O12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1159</v>
+      </c>
+      <c r="C2" t="s">
+        <v>479</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2">
+        <v>-4</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>F2/10+G2/5+H2/5+I2+J2+K2+L2+M2+N2</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>480</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="E3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>22</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O12" si="0">F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1161</v>
+      </c>
+      <c r="C4" t="s">
+        <v>481</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4">
+        <v>120</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>27</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>-5</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1162</v>
+      </c>
+      <c r="C5" t="s">
+        <v>482</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="E5" t="s">
+        <v>491</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>23</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>-4</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>F5/10+G5/5+H5/5+I5+J5+K5+L5+M5+N5+5*PowerRuling!G29</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1163</v>
+      </c>
+      <c r="C6" t="s">
+        <v>483</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="E6" t="s">
+        <v>490</v>
+      </c>
+      <c r="F6">
+        <v>140</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>40</v>
+      </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>8</v>
+      </c>
+      <c r="M6">
+        <v>-8</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>F6/10+G6/5+H6/5+I6+J6+K6+L6+M6+N6+1*8</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1164</v>
+      </c>
+      <c r="C7" t="s">
+        <v>492</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="E7" t="s">
+        <v>494</v>
+      </c>
+      <c r="F7">
+        <v>180</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>38</v>
+      </c>
+      <c r="J7">
+        <v>12</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>-5</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>F7/10+G7/5+H7/5+I7+J7+K7+L7+M7+N7+15</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1165</v>
+      </c>
+      <c r="C8" t="s">
+        <v>484</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E8" t="s">
+        <v>495</v>
+      </c>
+      <c r="F8">
+        <v>160</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>54</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>12</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>F8/10+G8/5+H8/5+I8+J8+K8+L8+M8+N8+1*8</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1166</v>
+      </c>
+      <c r="C9" t="s">
+        <v>508</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E9" t="s">
+        <v>501</v>
+      </c>
+      <c r="F9">
+        <v>150</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>50</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>16</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>F9/10+G9/5+H9/5+I9+J9+K9+L9+M9+N9+1*8</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1167</v>
+      </c>
+      <c r="C10" t="s">
+        <v>498</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="E10" t="s">
+        <v>500</v>
+      </c>
+      <c r="F10">
+        <v>300</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>80</v>
+      </c>
+      <c r="J10">
+        <v>15</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>15</v>
+      </c>
+      <c r="M10">
+        <v>-18</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>F10/10+G10/5+H10/5+I10+J10+K10+L10+M10+N10+1*8</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1168</v>
+      </c>
+      <c r="C11" t="s">
+        <v>502</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E11" t="s">
+        <v>504</v>
+      </c>
+      <c r="F11">
+        <v>270</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>82</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>35</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>F11/10+G11/5+H11/5+I11+J11+K11+L11+M11+N11+PowerRuling!L12</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1169</v>
+      </c>
+      <c r="C12" t="s">
+        <v>505</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E12" t="s">
+        <v>507</v>
+      </c>
+      <c r="F12">
+        <v>180</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>90</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12">
+        <v>20</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>F12/10+G12/5+H12/5+I12+J12+K12+L12+M12+N12+1*8+PowerRuling!G29*11</f>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9984AC-102E-4205-A4C3-1211F7E2ACAB}">
+  <dimension ref="B1:O23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1170</v>
+      </c>
+      <c r="C2" t="s">
+        <v>510</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>-7</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>F2/10+G2/5+H2/5+I2+J2+K2+L2+M2+N2+PowerRuling!$G$19*1+1*8+PowerRuling!L17</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1171</v>
+      </c>
+      <c r="C3" t="s">
+        <v>516</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>-9</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3+PowerRuling!$G$19*1+1*8+PowerRuling!L18</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1172</v>
+      </c>
+      <c r="C4" t="s">
+        <v>511</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="E4" t="s">
+        <v>532</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>-7</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>F4/10+G4/5+H4/5+I4+J4+K4+L4+M4+N4+PowerRuling!$G$19*2+1*8+PowerRuling!L17+PowerRuling!C61</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1173</v>
+      </c>
+      <c r="C5" t="s">
+        <v>515</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="E5" t="s">
+        <v>534</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>-9</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>F5/10+G5/5+H5/5+I5+J5+K5+L5+M5+N5+PowerRuling!$G$19*2+1*8+PowerRuling!L18+PowerRuling!C6</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1174</v>
+      </c>
+      <c r="C6" t="s">
+        <v>512</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="E6" t="s">
+        <v>251</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>16</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>-3</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>F6/10+G6/5+H6/5+I6+J6+K6+L6+M6+N6+PowerRuling!$G$19*3+PowerRuling!C62</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1175</v>
+      </c>
+      <c r="C7" t="s">
+        <v>521</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="E7" t="s">
+        <v>251</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>16</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>-5</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>F7/10+G7/5+H7/5+I7+J7+K7+L7+M7+N7+PowerRuling!$G$19*3+1*8+3*5</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1176</v>
+      </c>
+      <c r="C8" t="s">
+        <v>513</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="E8" t="s">
+        <v>539</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>21</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>-10</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>F8/10+G8/5+H8/5+I8+J8+K8+L8+M8+N8+PowerRuling!$G$19*4+PowerRuling!L17+1*8+PowerRuling!C61+8</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1177</v>
+      </c>
+      <c r="C9" t="s">
+        <v>524</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="E9" t="s">
+        <v>541</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>35</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>-8</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>F9/10+G9/5+H9/5+I9+J9+K9+L9+M9+N9+PowerRuling!$G$19*4+1*8+PowerRuling!L18+PowerRuling!C6</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1178</v>
+      </c>
+      <c r="C10" t="s">
+        <v>520</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>45</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10">
+        <v>-4</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>F10/10+G10/5+H10/5+I10+J10+K10+L10+M10+N10+PowerRuling!$G$19*5+PowerRuling!C19</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1179</v>
+      </c>
+      <c r="C11" t="s">
+        <v>543</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="E11" t="s">
+        <v>545</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>50</v>
+      </c>
+      <c r="J11">
+        <v>12</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>12</v>
+      </c>
+      <c r="M11">
+        <v>-14</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>F11/10+G11/5+H11/5+I11+J11+K11+L11+M11+N11+PowerRuling!$G$19*6+1*8+PowerRuling!L18+PowerRuling!C9+PowerRuling!C61</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1180</v>
+      </c>
+      <c r="C12" t="s">
+        <v>514</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="E12" t="s">
+        <v>547</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>60</v>
+      </c>
+      <c r="J12">
+        <v>12</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>12</v>
+      </c>
+      <c r="M12">
+        <v>-4</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>F12/10+G12/5+H12/5+I12+J12+K12+L12+M12+N12+PowerRuling!$G$19*6+1*8</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1181</v>
+      </c>
+      <c r="C13" t="s">
+        <v>536</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="E13" t="s">
+        <v>549</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>65</v>
+      </c>
+      <c r="J13">
+        <v>16</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>16</v>
+      </c>
+      <c r="M13">
+        <v>-14</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>F13/10+G13/5+H13/5+I13+J13+K13+L13+M13+N13+PowerRuling!$G$19*7+1*8+PowerRuling!C6+3*5</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1182</v>
+      </c>
+      <c r="C14" t="s">
+        <v>517</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="E14" t="s">
+        <v>551</v>
+      </c>
+      <c r="F14">
+        <v>100</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>70</v>
+      </c>
+      <c r="J14">
+        <v>22</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>22</v>
+      </c>
+      <c r="M14">
+        <v>-11</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>F14/10+G14/5+H14/5+I14+J14+K14+L14+M14+N14+PowerRuling!$G$19*8+1*8+PowerRuling!C19+PowerRuling!C6</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1183</v>
+      </c>
+      <c r="C15" t="s">
+        <v>525</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="E15" t="s">
+        <v>553</v>
+      </c>
+      <c r="F15">
+        <v>80</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>64</v>
+      </c>
+      <c r="J15">
+        <v>18</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>18</v>
+      </c>
+      <c r="M15">
+        <v>-8</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>F15/10+G15/5+H15/5+I15+J15+K15+L15+M15+N15+PowerRuling!$G$19*8+1*8+PowerRuling!L18+PowerRuling!C6+PowerRuling!C63</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1184</v>
+      </c>
+      <c r="C16" t="s">
+        <v>522</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="E16" t="s">
+        <v>555</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>70</v>
+      </c>
+      <c r="J16">
+        <v>15</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>15</v>
+      </c>
+      <c r="M16">
+        <v>-3</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>F16/10+G16/5+H16/5+I16+J16+K16+L16+M16+N16+PowerRuling!$G$19*8+PowerRuling!C9+PowerRuling!C62</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1185</v>
+      </c>
+      <c r="C17" t="s">
+        <v>556</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="E17" t="s">
+        <v>558</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>85</v>
+      </c>
+      <c r="J17">
+        <v>12</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>12</v>
+      </c>
+      <c r="M17">
+        <v>17</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>F17/10+G17/5+H17/5+I17+J17+K17+L17+M17+N17+PowerRuling!$G$19*9+2*8+PowerRuling!L20</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1186</v>
+      </c>
+      <c r="C18" t="s">
+        <v>519</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="E18" t="s">
+        <v>560</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>91</v>
+      </c>
+      <c r="J18">
+        <v>16</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>16</v>
+      </c>
+      <c r="M18">
+        <v>-4</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>F18/10+G18/5+H18/5+I18+J18+K18+L18+M18+N18+PowerRuling!$G$19*9+1*8+PowerRuling!L17+PowerRuling!C61+PowerRuling!C9+PowerRuling!C64</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1187</v>
+      </c>
+      <c r="C19" t="s">
+        <v>527</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="E19" t="s">
+        <v>562</v>
+      </c>
+      <c r="F19">
+        <v>200</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>95</v>
+      </c>
+      <c r="J19">
+        <v>24</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>24</v>
+      </c>
+      <c r="M19">
+        <v>-16</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f>F19/10+G19/5+H19/5+I19+J19+K19+L19+M19+N19+PowerRuling!$G$19*10+1*8+3*5+PowerRuling!L17+PowerRuling!C6</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1188</v>
+      </c>
+      <c r="C20" t="s">
+        <v>523</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="E20" t="s">
+        <v>564</v>
+      </c>
+      <c r="F20">
+        <v>150</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>95</v>
+      </c>
+      <c r="J20">
+        <v>20</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>20</v>
+      </c>
+      <c r="M20">
+        <v>-5</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f>F20/10+G20/5+H20/5+I20+J20+K20+L20+M20+N20+PowerRuling!$G$19*10+PowerRuling!C62+1*8+PowerRuling!C9</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1189</v>
+      </c>
+      <c r="C21" t="s">
+        <v>518</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="E21" t="s">
+        <v>566</v>
+      </c>
+      <c r="F21">
+        <v>100</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>85</v>
+      </c>
+      <c r="J21">
+        <v>34</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>34</v>
+      </c>
+      <c r="M21">
+        <v>-20</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f>F21/10+G21/5+H21/5+I21+J21+K21+L21+M21+N21+PowerRuling!$G$19*11+1*8+4*8+3*5+PowerRuling!C6</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1190</v>
+      </c>
+      <c r="C22" t="s">
+        <v>528</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="E22" t="s">
+        <v>568</v>
+      </c>
+      <c r="F22">
+        <v>300</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>85</v>
+      </c>
+      <c r="J22">
+        <v>30</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>30</v>
+      </c>
+      <c r="M22">
+        <v>-11</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>F22/10+G22/5+H22/5+I22+J22+K22+L22+M22+N22+PowerRuling!$G$19*11+1*8+PowerRuling!C6+PowerRuling!C9+PowerRuling!C19+PowerRuling!L17+PowerRuling!C61</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1191</v>
+      </c>
+      <c r="C23" t="s">
+        <v>526</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="E23" t="s">
+        <v>570</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>110</v>
+      </c>
+      <c r="J23">
+        <v>16</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>16</v>
+      </c>
+      <c r="M23">
+        <v>25</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>F23/10+G23/5+H23/5+I23+J23+K23+L23+M23+N23+PowerRuling!$G$19*12+3*8+PowerRuling!L20+PowerRuling!L17+PowerRuling!C9+PowerRuling!C64+PowerRuling!C61</f>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD9F617-3516-4490-8C9F-43ED117A1264}">
+  <dimension ref="B1:O15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="5" max="5" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1192</v>
+      </c>
+      <c r="C2" t="s">
+        <v>583</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="E2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>8</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>F2/10+G2/5+H2/5+I2+J2+K2+L2+M2+N2+PowerRuling!C13</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1193</v>
+      </c>
+      <c r="C3" t="s">
+        <v>572</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="E3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>25</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3+PowerRuling!L8</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1194</v>
+      </c>
+      <c r="C4" t="s">
+        <v>586</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>F4/10+G4/5+H4/5+I4+J4+K4+L4+M4+N4+1*8+PowerRuling!C6</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1195</v>
+      </c>
+      <c r="C5" t="s">
+        <v>573</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="E5" t="s">
+        <v>589</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>8</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>F5/10+G5/5+H5/5+I5+J5+K5+L5+M5+N5+PowerRuling!C13+PowerRuling!C16</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1196</v>
+      </c>
+      <c r="C6" t="s">
+        <v>574</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="E6" t="s">
+        <v>591</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>18</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>F6/10+G6/5+H6/5+I6+J6+K6+L6+M6+N6+PowerRuling!L8+PowerRuling!C13</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1197</v>
+      </c>
+      <c r="C7" t="s">
+        <v>575</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="E7" t="s">
+        <v>593</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>17</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>F7/10+G7/5+H7/5+I7+J7+K7+L7+M7+N7+1*8+PowerRuling!C7</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1198</v>
+      </c>
+      <c r="C8" t="s">
+        <v>577</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="E8" t="s">
+        <v>595</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>60</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>16</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>34</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>F8/10+G8/5+H8/5+I8+J8+K8+L8+M8+N8+PowerRuling!C14+PowerRuling!C17</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1199</v>
+      </c>
+      <c r="C9" t="s">
+        <v>578</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="E9" t="s">
+        <v>597</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>85</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>22</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>45</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>F9/10+G9/5+H9/5+I9+J9+K9+L9+M9+N9+PowerRuling!L8+PowerRuling!C15</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1200</v>
+      </c>
+      <c r="C10" t="s">
+        <v>582</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="E10" t="s">
+        <v>599</v>
+      </c>
+      <c r="F10">
+        <v>70</v>
+      </c>
+      <c r="G10">
+        <v>60</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>20</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>45</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>F10/10+G10/5+H10/5+I10+J10+K10+L10+M10+N10+1*8+PowerRuling!C7+PowerRuling!C19</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1201</v>
+      </c>
+      <c r="C11" t="s">
+        <v>579</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="E11" t="s">
+        <v>601</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>27</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>50</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>F11/10+G11/5+H11/5+I11+J11+K11+L11+M11+N11+PowerRuling!C14+PowerRuling!C17+PowerRuling!L8</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1202</v>
+      </c>
+      <c r="C12" t="s">
+        <v>602</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="E12" t="s">
+        <v>558</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>50</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>37</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>37</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>F12/10+G12/5+H12/5+I12+J12+K12+L12+M12+N12+1*8+PowerRuling!C7+PowerRuling!C20+PowerRuling!C14</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1203</v>
+      </c>
+      <c r="C13" t="s">
+        <v>580</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="E13" t="s">
+        <v>605</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>125</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>35</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>65</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>F13/10+G13/5+H13/5+I13+J13+K13+L13+M13+N13+5*3+PowerRuling!L8*2</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1204</v>
+      </c>
+      <c r="C14" t="s">
+        <v>581</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="E14" t="s">
+        <v>607</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>80</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>45</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>55</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>F14/10+G14/5+H14/5+I14+J14+K14+L14+M14+N14+PowerRuling!C7+PowerRuling!C14+PowerRuling!C20+2*8</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1205</v>
+      </c>
+      <c r="C15" t="s">
+        <v>576</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="E15" t="s">
+        <v>609</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>130</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>35</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>72</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>F15/10+G15/5+H15/5+I15+J15+K15+L15+M15+N15+5*3+2*PowerRuling!L8+PowerRuling!C15+PowerRuling!C18</f>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3125C839-1A13-4135-8FE2-BA0C0DD834FF}">
+  <dimension ref="B1:O11"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1206</v>
+      </c>
+      <c r="C2" t="s">
+        <v>613</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>25</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>6</v>
+      </c>
+      <c r="O2">
+        <f>F2/10+G2/5+H2/5+I2+J2+K2+L2+M2+N2</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1207</v>
+      </c>
+      <c r="C3" t="s">
+        <v>612</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>32</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O11" si="0">F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1208</v>
+      </c>
+      <c r="C4" t="s">
+        <v>611</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="E4" t="s">
+        <v>623</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>40</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>11</v>
+      </c>
+      <c r="O4">
+        <f>F4/10+G4/5+H4/5+I4+J4+K4+L4+M4+N4+PowerRuling!C13</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1209</v>
+      </c>
+      <c r="C5" t="s">
+        <v>614</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>40</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>55</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>-15</v>
+      </c>
+      <c r="N5">
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <f>F5/10+G5/5+H5/5+I5+J5+K5+L5+M5+N5+20</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1210</v>
+      </c>
+      <c r="C6" t="s">
+        <v>625</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="E6" t="s">
+        <v>626</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>80</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>45</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>12</v>
+      </c>
+      <c r="N6">
+        <v>12</v>
+      </c>
+      <c r="O6">
+        <f>F6/10+G6/5+H6/5+I6+J6+K6+L6+M6+N6+PowerRuling!C6</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1211</v>
+      </c>
+      <c r="C7" t="s">
+        <v>615</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="E7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>35</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>6</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <f>F7/10+G7/5+H7/5+I7+J7+K7+L7+M7+N7+1*8+PowerRuling!G29*7</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1212</v>
+      </c>
+      <c r="C8" t="s">
+        <v>616</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="E8" t="s">
+        <v>629</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>60</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>70</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>-22</v>
+      </c>
+      <c r="N8">
+        <v>10</v>
+      </c>
+      <c r="O8">
+        <f>F8/10+G8/5+H8/5+I8+J8+K8+L8+M8+N8+20</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1213</v>
+      </c>
+      <c r="C9" t="s">
+        <v>617</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="E9" t="s">
+        <v>629</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>40</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>70</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>-18</v>
+      </c>
+      <c r="N9">
+        <v>10</v>
+      </c>
+      <c r="O9">
+        <f>F9/10+G9/5+H9/5+I9+J9+K9+L9+M9+N9+20</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1214</v>
+      </c>
+      <c r="C10" t="s">
+        <v>618</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="E10" t="s">
+        <v>632</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>80</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>70</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>16</v>
+      </c>
+      <c r="O10">
+        <f>F10/10+G10/5+H10/5+I10+J10+K10+L10+M10+N10+PowerRuling!C14+PowerRuling!C17</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1215</v>
+      </c>
+      <c r="C11" t="s">
+        <v>619</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="E11" t="s">
+        <v>635</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>80</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>90</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>17</v>
+      </c>
+      <c r="N11">
+        <v>17</v>
+      </c>
+      <c r="O11">
+        <f>F11/10+G11/5+H11/5+I11+J11+K11+L11+M11+N11+PowerRuling!C7+20</f>
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79A045F-B925-432F-BC47-D75FF4A11A33}">
+  <dimension ref="B1:O10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="5" max="5" width="73.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G1" t="s">
+        <v>668</v>
+      </c>
+      <c r="H1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I1" t="s">
+        <v>670</v>
+      </c>
+      <c r="J1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K1" t="s">
+        <v>672</v>
+      </c>
+      <c r="L1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M1" t="s">
+        <v>674</v>
+      </c>
+      <c r="N1" t="s">
+        <v>675</v>
+      </c>
+      <c r="O1" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1216</v>
+      </c>
+      <c r="C2" t="s">
+        <v>638</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>F2/10+G2/5+H2/5+I2+J2+K2+L2+M2+N2+PowerRuling!$G$19*2</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1217</v>
+      </c>
+      <c r="C3" t="s">
+        <v>639</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="E3" t="s">
+        <v>659</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>13</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3+PowerRuling!$G$19*3+PowerRuling!C65</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1218</v>
+      </c>
+      <c r="C4" t="s">
+        <v>640</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="E4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F4">
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>F4/10+G4/5+H4/5+I4+J4+K4+L4+M4+N4+PowerRuling!$G$19*3+1*8+PowerRuling!L8</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1219</v>
+      </c>
+      <c r="C5" t="s">
+        <v>641</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="E5" t="s">
+        <v>251</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>40</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>8</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>F5/10+G5/5+H5/5+I5+J5+K5+L5+M5+N5+PowerRuling!$G$19*3+1*8+PowerRuling!L8</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1220</v>
+      </c>
+      <c r="C6" t="s">
+        <v>642</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="E6" t="s">
+        <v>650</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>F6/10+G6/5+H6/5+I6+J6+K6+L6+M6+N6+PowerRuling!$G$19*5+1*8+PowerRuling!C65+14</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1221</v>
+      </c>
+      <c r="C7" t="s">
+        <v>643</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="E7" t="s">
+        <v>652</v>
+      </c>
+      <c r="F7">
+        <v>80</v>
+      </c>
+      <c r="G7">
+        <v>80</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>18</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>48</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>F7/10+G7/5+H7/5+I7+J7+K7+L7+M7+N7+PowerRuling!$G$19*7+2*8+PowerRuling!L8</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1222</v>
+      </c>
+      <c r="C8" t="s">
+        <v>644</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="E8" t="s">
+        <v>655</v>
+      </c>
+      <c r="F8">
+        <v>120</v>
+      </c>
+      <c r="G8">
+        <v>160</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>35</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>80</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>F8/10+G8/5+H8/5+I8+J8+K8+L8+M8+N8+PowerRuling!$G$19*10+1*8+3+PowerRuling!L14</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1223</v>
+      </c>
+      <c r="C9" t="s">
+        <v>645</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="E9" t="s">
+        <v>655</v>
+      </c>
+      <c r="F9">
+        <v>80</v>
+      </c>
+      <c r="G9">
+        <v>160</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>25</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>90</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>F9/10+G9/5+H9/5+I9+J9+K9+L9+M9+N9+PowerRuling!$G$19*10+3*1+1*8+PowerRuling!G33</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1224</v>
+      </c>
+      <c r="C10" t="s">
+        <v>636</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="E10" t="s">
+        <v>658</v>
+      </c>
+      <c r="F10">
+        <v>120</v>
+      </c>
+      <c r="G10">
+        <v>160</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>46</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>100</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>F10/10+G10/5+H10/5+I10+J10+K10+L10+M10+N10+PowerRuling!$G$19*12+6+2*8+PowerRuling!G33+PowerRuling!L14</f>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B5F246-E8D7-402E-9A8B-F3ABB3622514}">
-  <dimension ref="B2:L60"/>
+  <dimension ref="B2:L65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8030,7 +11294,7 @@
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="G14">
         <v>12</v>
@@ -8067,7 +11331,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>691</v>
       </c>
@@ -8080,16 +11344,28 @@
       <c r="G17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>755</v>
+      </c>
+      <c r="L17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>692</v>
       </c>
       <c r="C18">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>756</v>
+      </c>
+      <c r="L18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>696</v>
       </c>
@@ -8097,21 +11373,27 @@
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G19">
         <v>-3</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>697</v>
       </c>
       <c r="C20">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>760</v>
+      </c>
+      <c r="L20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>698</v>
       </c>
@@ -8119,7 +11401,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>726</v>
       </c>
@@ -8130,7 +11412,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>693</v>
       </c>
@@ -8141,7 +11423,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>694</v>
       </c>
@@ -8149,7 +11431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>695</v>
       </c>
@@ -8157,7 +11439,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>699</v>
       </c>
@@ -8168,7 +11450,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>700</v>
       </c>
@@ -8176,10 +11458,10 @@
         <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>706</v>
       </c>
@@ -8187,7 +11469,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>707</v>
       </c>
@@ -8195,13 +11477,13 @@
         <v>8</v>
       </c>
       <c r="F29" t="s">
-        <v>731</v>
+        <v>754</v>
       </c>
       <c r="G29">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>708</v>
       </c>
@@ -8209,7 +11491,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>709</v>
       </c>
@@ -8217,10 +11499,10 @@
         <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>711</v>
       </c>
@@ -8228,7 +11510,7 @@
         <v>22</v>
       </c>
       <c r="F32" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G32">
         <v>14</v>
@@ -8242,7 +11524,7 @@
         <v>7</v>
       </c>
       <c r="F33" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="G33">
         <v>14</v>
@@ -8330,7 +11612,7 @@
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C44">
         <v>11</v>
@@ -8338,7 +11620,7 @@
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C45">
         <v>13</v>
@@ -8346,7 +11628,7 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C46">
         <v>14</v>
@@ -8354,7 +11636,7 @@
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C47">
         <v>8</v>
@@ -8362,7 +11644,7 @@
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="C48">
         <v>14</v>
@@ -8370,7 +11652,7 @@
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C49">
         <v>10</v>
@@ -8378,7 +11660,7 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C50">
         <v>15</v>
@@ -8386,7 +11668,7 @@
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C51">
         <v>8</v>
@@ -8394,7 +11676,7 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C52">
         <v>12</v>
@@ -8402,7 +11684,7 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C53">
         <v>7</v>
@@ -8410,7 +11692,7 @@
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C54">
         <v>15</v>
@@ -8418,7 +11700,7 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C55">
         <v>6</v>
@@ -8426,7 +11708,7 @@
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C56">
         <v>6</v>
@@ -8434,7 +11716,7 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C57">
         <v>11</v>
@@ -8442,7 +11724,7 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C58">
         <v>12</v>
@@ -8450,7 +11732,7 @@
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C59">
         <v>15</v>
@@ -8458,10 +11740,50 @@
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C60">
         <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>757</v>
+      </c>
+      <c r="C61">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>758</v>
+      </c>
+      <c r="C62">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>759</v>
+      </c>
+      <c r="C63">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>761</v>
+      </c>
+      <c r="C64">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>762</v>
+      </c>
+      <c r="C65">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Toutes les stats sont encodées dans le XML
</commit_message>
<xml_diff>
--- a/Documentation/Items.xlsx
+++ b/Documentation/Items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxad\Documents\git_projects\LC_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833E0524-D585-4BFA-9920-9FFC57AD48AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D234157-381C-4B7B-B38F-CA818595A14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="696" activeTab="14" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="696" firstSheet="9" activeTab="14" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
   </bookViews>
   <sheets>
     <sheet name="ListOfItems" sheetId="1" r:id="rId1"/>
@@ -6810,8 +6810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B29AA04-5439-44D8-B921-81D0FBC20718}">
   <dimension ref="B1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:O1"/>
+    <sheetView topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7916,8 +7916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34650302-33EE-4E55-BC98-54EF095D0F8E}">
   <dimension ref="B1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:O1"/>
+    <sheetView topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8046,7 +8046,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O12" si="0">F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3</f>
+        <f t="shared" ref="O3:O4" si="0">F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3</f>
         <v>25</v>
       </c>
     </row>
@@ -8464,8 +8464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9984AC-102E-4205-A4C3-1211F7E2ACAB}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:O1"/>
+    <sheetView topLeftCell="E20" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9507,7 +9507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD9F617-3516-4490-8C9F-43ED117A1264}">
   <dimension ref="B1:O15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="E11" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -10190,7 +10190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3125C839-1A13-4135-8FE2-BA0C0DD834FF}">
   <dimension ref="B1:O11"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="E7" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -10320,7 +10320,7 @@
         <v>6</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O11" si="0">F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3</f>
+        <f t="shared" ref="O3" si="0">F3/10+G3/5+H3/5+I3+J3+K3+L3+M3+N3</f>
         <v>50</v>
       </c>
     </row>
@@ -10693,7 +10693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79A045F-B925-432F-BC47-D75FF4A11A33}">
   <dimension ref="B1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
       <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
@@ -11795,8 +11795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFDFD57-C829-46C4-A7CF-3734419064E7}">
   <dimension ref="B1:O33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:O1"/>
+    <sheetView topLeftCell="E26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13257,8 +13257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A67A6C-BD76-4F63-B522-FA55F75B46B2}">
   <dimension ref="B1:O22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:O1"/>
+    <sheetView topLeftCell="E15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13642,10 +13642,10 @@
         <v>6</v>
       </c>
       <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>5</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -13822,10 +13822,10 @@
         <v>11</v>
       </c>
       <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>14</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -14137,10 +14137,10 @@
         <v>23</v>
       </c>
       <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
         <v>55</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -14224,7 +14224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71C5CED-70F3-4061-8153-EB3DDD81F3FA}">
   <dimension ref="B1:O19"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E15" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -15059,8 +15059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52245DA4-B6A7-43F4-9E25-B651EFDB9442}">
   <dimension ref="B1:O15"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="E9" workbookViewId="0">
+      <selection activeCell="B12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15742,7 +15742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09AA25AD-0CA4-48E8-92CF-38BBD575942E}">
   <dimension ref="B1:O24"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="E19" workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
@@ -16830,8 +16830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77D27EC-A5E9-4AC1-8ACA-52AFB6B78A4C}">
   <dimension ref="B1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:O1"/>
+    <sheetView topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17558,7 +17558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584D62A5-C004-44A9-885B-19FEC1A55407}">
   <dimension ref="B1:O13"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="E9" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Encodage des items consommables dans les XML
</commit_message>
<xml_diff>
--- a/Documentation/Items.xlsx
+++ b/Documentation/Items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity_Projects\LC_Unity\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxad\Documents\git_projects\LC_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3B7072-B8BD-4568-A0A7-10EB11AE94BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72EF5167-99C8-4E5C-BBD3-2CA4571C5991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="696" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="696" xr2:uid="{EA6D107C-C583-4F45-9DA7-DCFEC8078555}"/>
   </bookViews>
   <sheets>
     <sheet name="ListOfItems" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="858">
   <si>
     <t>ID</t>
   </si>
@@ -2621,6 +2621,9 @@
   </si>
   <si>
     <t>Grants additional Defense and Magic Defense, but reduces Accuracy.</t>
+  </si>
+  <si>
+    <t>Restores 100% of the target's max Mana.</t>
   </si>
 </sst>
 </file>
@@ -2997,8 +3000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE263883-2701-4B73-BA24-C20413007C34}">
   <dimension ref="B2:F292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3079,7 +3082,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>857</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">

</xml_diff>